<commit_message>
fix: kobo link in info popup AB#18547
</commit_message>
<xml_diff>
--- a/services/API-service/src/scripts/json/layer-popup-info.xlsx
+++ b/services/API-service/src/scripts/json/layer-popup-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\services\API-service\src\scripts\json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF138E9-ECB6-40D1-B50D-6AF7C3A2E596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6DA600-603A-4932-BA18-3D3834337217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
+    <workbookView xWindow="15195" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1449,7 +1449,7 @@
     <t>community_notifications</t>
   </si>
   <si>
-    <t>Community notifications are sent via volunteers that have direct contact with the community. They assess the information and fill in the details in a digital form.&lt;br&gt;&lt;br&gt;The notifications are visualized as drop pins with a bell icon on the map.&lt;br&gt;&lt;br&gt;&lt;strong&gt;What to do?&lt;/strong&gt; Click on the drop pin to open it and see the information attached to it. Some notifications contain photos.&lt;br&gt;&lt;br&gt;The pins on the map will stay on the map until manually deleted. Make sure to delete irrelevant and old notifications.&lt;br&gt;&lt;br&gt;&lt;strong&gt;All sent notifications including deleted ones&lt;/strong&gt;: https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx.</t>
+    <t>Community notifications are sent via volunteers that have direct contact with the community. They assess the information and fill in the details in a digital form.&lt;br&gt;&lt;br&gt;The notifications are visualized as drop pins with a bell icon on the map.&lt;br&gt;&lt;br&gt;&lt;strong&gt;What to do?&lt;/strong&gt; Click on the drop pin to open it and see the information attached to it. Some notifications contain photos.&lt;br&gt;&lt;br&gt;The pins on the map will stay on the map until manually deleted. Make sure to delete irrelevant and old notifications.&lt;br&gt;&lt;br&gt;&lt;strong&gt;All sent notifications including deleted ones&lt;/strong&gt;: &lt;a href='https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx'&gt;https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -1962,8 +1962,8 @@
   <dimension ref="A1:S429"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2043,47 +2043,47 @@
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="14" t="str">
-        <f t="shared" ref="I2:I22" si="0">IF(A1="section","{","")</f>
+        <f t="shared" ref="I2" si="0">IF(A1="section","{","")</f>
         <v>{</v>
       </c>
       <c r="J2" s="13" t="str">
-        <f t="shared" ref="J2:J22" si="1">IF(A2=A1,"",""""&amp;A2&amp;""": {")</f>
+        <f t="shared" ref="J2" si="1">IF(A2=A1,"",""""&amp;A2&amp;""": {")</f>
         <v>"layers-section": {</v>
       </c>
       <c r="K2" s="13" t="str">
-        <f t="shared" ref="K2:K22" si="2">IF(B2=B1,"",""""&amp;B2&amp;""": {")</f>
+        <f t="shared" ref="K2" si="2">IF(B2=B1,"",""""&amp;B2&amp;""": {")</f>
         <v>"affected_population": {</v>
       </c>
       <c r="L2" s="25" t="str">
-        <f t="shared" ref="L2:L22" si="3">IF(AND(B2=B1,C2=C1),"",""""&amp;C2&amp;""": {")</f>
+        <f t="shared" ref="L2" si="3">IF(AND(B2=B1,C2=C1),"",""""&amp;C2&amp;""": {")</f>
         <v>"PHL": {</v>
       </c>
       <c r="M2" s="13" t="str">
-        <f t="shared" ref="M2:M22" si="4">""""&amp;D2&amp;""": """&amp;SUBSTITUTE(G2,"""","'")&amp;""""</f>
+        <f t="shared" ref="M2" si="4">""""&amp;D2&amp;""": """&amp;SUBSTITUTE(G2,"""","'")&amp;""""</f>
         <v>"typhoon": "&lt;p&gt;The number of people affected is calculated based on the predicted number of completely damaged houses, which is derived from the typhoon impact predicting model. To derive a methodology to estimate the number of affected people from a predicted number of completely damaged houses, we performed a log fit between the number of completely damaged houses and the number of affected people for past typhoon events using data derived from DROMIC reports. To estimate potential number of affected population this formula is applied to the predicted number of damaged houses. &lt;p&gt; "</v>
       </c>
       <c r="N2" s="26" t="str">
-        <f t="shared" ref="N2:N22" si="5">IF(AND(B3=B2,C3=C2),",","}")</f>
+        <f t="shared" ref="N2" si="5">IF(AND(B3=B2,C3=C2),",","}")</f>
         <v>}</v>
       </c>
       <c r="O2" s="13" t="str">
-        <f t="shared" ref="O2:O22" si="6">IF(NOT(B2=B3),"}",IF(C2=C3,"",","))</f>
+        <f t="shared" ref="O2" si="6">IF(NOT(B2=B3),"}",IF(C2=C3,"",","))</f>
         <v>}</v>
       </c>
       <c r="P2" s="13" t="str">
-        <f t="shared" ref="P2:P22" si="7">IF(B2=B3,"",IF(A2=A3,",",""))</f>
+        <f t="shared" ref="P2" si="7">IF(B2=B3,"",IF(A2=A3,",",""))</f>
         <v>,</v>
       </c>
       <c r="Q2" s="13" t="str">
-        <f t="shared" ref="Q2:Q22" si="8">IF(A3=A2,"",IF(A3="","}","},"))</f>
+        <f t="shared" ref="Q2" si="8">IF(A3=A2,"",IF(A3="","}","},"))</f>
         <v/>
       </c>
       <c r="R2" s="13" t="str">
-        <f t="shared" ref="R2:R22" si="9">IF(A3="","}","")</f>
+        <f t="shared" ref="R2" si="9">IF(A3="","}","")</f>
         <v/>
       </c>
       <c r="S2" s="13" t="str">
-        <f t="shared" ref="S2:S22" si="10">IF(A2="","",I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2&amp;P2&amp;Q2&amp;R2)</f>
+        <f t="shared" ref="S2" si="10">IF(A2="","",I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2&amp;P2&amp;Q2&amp;R2)</f>
         <v>{"layers-section": {"affected_population": {"PHL": {"typhoon": "&lt;p&gt;The number of people affected is calculated based on the predicted number of completely damaged houses, which is derived from the typhoon impact predicting model. To derive a methodology to estimate the number of affected people from a predicted number of completely damaged houses, we performed a log fit between the number of completely damaged houses and the number of affected people for past typhoon events using data derived from DROMIC reports. To estimate potential number of affected population this formula is applied to the predicted number of damaged houses. &lt;p&gt; "}},</v>
       </c>
     </row>
@@ -3435,7 +3435,7 @@
         <v>"cattle_exposed": {"ZWE": {"drought": "&lt;p&gt;Number of exposed cattle is calculated by the cattle per province within the droughts alert threshold reached area currently triggered. Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 as reference unit, which is the grazing equivalent of one adult dairy cow producing 3000 kg of milk annually, without additional concentrated foodstuffs.&amp;nbsp;&lt;/p&gt;&lt;p&gt;Source Links :&lt;/p&gt; &lt;ul&gt;     &lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021.&lt;/li&gt;     &lt;li&gt;Source assessment:&lt;br&gt;&lt;a target='_blank' data-fr-linked='true' href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;&lt;/li&gt;     &lt;li&gt;Source Livestock unit (LSU) &lt;a target='_blank' href='https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)'&gt;&amp;nbsp;https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)&lt;/a&gt;&lt;/li&gt; &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="9" t="s">
         <v>116</v>
       </c>
@@ -3472,7 +3472,7 @@
       </c>
       <c r="M23" s="13" t="str">
         <f t="shared" si="15"/>
-        <v>"heavy-rain": "Community notifications are sent via volunteers that have direct contact with the community. They assess the information and fill in the details in a digital form.&lt;br&gt;&lt;br&gt;The notifications are visualized as drop pins with a bell icon on the map.&lt;br&gt;&lt;br&gt;&lt;strong&gt;What to do?&lt;/strong&gt; Click on the drop pin to open it and see the information attached to it. Some notifications contain photos.&lt;br&gt;&lt;br&gt;The pins on the map will stay on the map until manually deleted. Make sure to delete irrelevant and old notifications.&lt;br&gt;&lt;br&gt;&lt;strong&gt;All sent notifications including deleted ones&lt;/strong&gt;: https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx."</v>
+        <v>"heavy-rain": "Community notifications are sent via volunteers that have direct contact with the community. They assess the information and fill in the details in a digital form.&lt;br&gt;&lt;br&gt;The notifications are visualized as drop pins with a bell icon on the map.&lt;br&gt;&lt;br&gt;&lt;strong&gt;What to do?&lt;/strong&gt; Click on the drop pin to open it and see the information attached to it. Some notifications contain photos.&lt;br&gt;&lt;br&gt;The pins on the map will stay on the map until manually deleted. Make sure to delete irrelevant and old notifications.&lt;br&gt;&lt;br&gt;&lt;strong&gt;All sent notifications including deleted ones&lt;/strong&gt;: &lt;a href='https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx'&gt;https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx&lt;/a&gt;"</v>
       </c>
       <c r="N23" s="26" t="str">
         <f t="shared" si="16"/>
@@ -3496,7 +3496,7 @@
       </c>
       <c r="S23" s="13" t="str">
         <f t="shared" si="21"/>
-        <v>"community_notifications": {"UGA": {"heavy-rain": "Community notifications are sent via volunteers that have direct contact with the community. They assess the information and fill in the details in a digital form.&lt;br&gt;&lt;br&gt;The notifications are visualized as drop pins with a bell icon on the map.&lt;br&gt;&lt;br&gt;&lt;strong&gt;What to do?&lt;/strong&gt; Click on the drop pin to open it and see the information attached to it. Some notifications contain photos.&lt;br&gt;&lt;br&gt;The pins on the map will stay on the map until manually deleted. Make sure to delete irrelevant and old notifications.&lt;br&gt;&lt;br&gt;&lt;strong&gt;All sent notifications including deleted ones&lt;/strong&gt;: https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx."}},</v>
+        <v>"community_notifications": {"UGA": {"heavy-rain": "Community notifications are sent via volunteers that have direct contact with the community. They assess the information and fill in the details in a digital form.&lt;br&gt;&lt;br&gt;The notifications are visualized as drop pins with a bell icon on the map.&lt;br&gt;&lt;br&gt;&lt;strong&gt;What to do?&lt;/strong&gt; Click on the drop pin to open it and see the information attached to it. Some notifications contain photos.&lt;br&gt;&lt;br&gt;The pins on the map will stay on the map until manually deleted. Make sure to delete irrelevant and old notifications.&lt;br&gt;&lt;br&gt;&lt;strong&gt;All sent notifications including deleted ones&lt;/strong&gt;: &lt;a href='https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx'&gt;https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx&lt;/a&gt;"}},</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="144" x14ac:dyDescent="0.55000000000000004">
@@ -21607,47 +21607,47 @@
       <c r="G310" s="6"/>
       <c r="H310" s="19"/>
       <c r="I310" s="14" t="str">
-        <f t="shared" ref="I261:I324" si="66">IF(A309="section","{","")</f>
+        <f t="shared" ref="I310:I324" si="66">IF(A309="section","{","")</f>
         <v/>
       </c>
       <c r="J310" s="13" t="str">
-        <f t="shared" ref="J261:J324" si="67">IF(A310=A309,"",""""&amp;A310&amp;""": {")</f>
+        <f t="shared" ref="J310:J324" si="67">IF(A310=A309,"",""""&amp;A310&amp;""": {")</f>
         <v/>
       </c>
       <c r="K310" s="13" t="str">
-        <f t="shared" ref="K261:K324" si="68">IF(B310=B309,"",""""&amp;B310&amp;""": {")</f>
+        <f t="shared" ref="K310:K324" si="68">IF(B310=B309,"",""""&amp;B310&amp;""": {")</f>
         <v/>
       </c>
       <c r="L310" s="25" t="str">
-        <f t="shared" ref="L261:L324" si="69">IF(AND(B310=B309,C310=C309),"",""""&amp;C310&amp;""": {")</f>
+        <f t="shared" ref="L310:L324" si="69">IF(AND(B310=B309,C310=C309),"",""""&amp;C310&amp;""": {")</f>
         <v/>
       </c>
       <c r="M310" s="13" t="str">
-        <f t="shared" ref="M280:M343" si="70">""""&amp;D310&amp;""": """&amp;SUBSTITUTE(G310,"""","'")&amp;""""</f>
+        <f t="shared" ref="M310:M343" si="70">""""&amp;D310&amp;""": """&amp;SUBSTITUTE(G310,"""","'")&amp;""""</f>
         <v>"": ""</v>
       </c>
       <c r="N310" s="26" t="str">
-        <f t="shared" ref="N260:N323" si="71">IF(AND(B311=B310,C311=C310),",","}")</f>
+        <f t="shared" ref="N310:N323" si="71">IF(AND(B311=B310,C311=C310),",","}")</f>
         <v>,</v>
       </c>
       <c r="O310" s="13" t="str">
-        <f t="shared" ref="O260:O323" si="72">IF(NOT(B310=B311),"}",IF(C310=C311,"",","))</f>
+        <f t="shared" ref="O310:O323" si="72">IF(NOT(B310=B311),"}",IF(C310=C311,"",","))</f>
         <v/>
       </c>
       <c r="P310" s="13" t="str">
-        <f t="shared" ref="P260:P323" si="73">IF(B310=B311,"",IF(A310=A311,",",""))</f>
+        <f t="shared" ref="P310:P323" si="73">IF(B310=B311,"",IF(A310=A311,",",""))</f>
         <v/>
       </c>
       <c r="Q310" s="13" t="str">
-        <f t="shared" ref="Q260:Q323" si="74">IF(A311=A310,"",IF(A311="","}","},"))</f>
+        <f t="shared" ref="Q310:Q323" si="74">IF(A311=A310,"",IF(A311="","}","},"))</f>
         <v/>
       </c>
       <c r="R310" s="13" t="str">
-        <f t="shared" ref="R260:R323" si="75">IF(A311="","}","")</f>
+        <f t="shared" ref="R310:R323" si="75">IF(A311="","}","")</f>
         <v>}</v>
       </c>
       <c r="S310" s="13" t="str">
-        <f t="shared" ref="S280:S343" si="76">IF(A310="","",I310&amp;J310&amp;K310&amp;L310&amp;M310&amp;N310&amp;O310&amp;P310&amp;Q310&amp;R310)</f>
+        <f t="shared" ref="S310:S343" si="76">IF(A310="","",I310&amp;J310&amp;K310&amp;L310&amp;M310&amp;N310&amp;O310&amp;P310&amp;Q310&amp;R310)</f>
         <v/>
       </c>
     </row>
@@ -26939,7 +26939,7 @@
         <v>}</v>
       </c>
       <c r="S408" s="13" t="str">
-        <f t="shared" ref="S408:S471" si="98">IF(A408="","",I408&amp;J408&amp;K408&amp;L408&amp;M408&amp;N408&amp;O408&amp;P408&amp;Q408&amp;R408)</f>
+        <f t="shared" ref="S408:S429" si="98">IF(A408="","",I408&amp;J408&amp;K408&amp;L408&amp;M408&amp;N408&amp;O408&amp;P408&amp;Q408&amp;R408)</f>
         <v/>
       </c>
     </row>
@@ -28070,7 +28070,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DbwGjqDGrfCW1GnpF6cxRqrWWp3rgn5Isr5GpVZi9tmwONwCM0F5vQCl5rOLn8rp2swjaeNqjzpZtwpk9q1BWg==" saltValue="EwiXw5LQI9vcmIa3pxbhgg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="/2cQJi+i8cAZdTOEtvA14sKUkbKkCfiNOt5+1emBF3SA7mHaD944VfbOvqD121Wkbo/0g52ddVMadxgrCkXx0A==" saltValue="3UdpGa7ferffexeCF0WtDA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>

</xml_diff>

<commit_message>
fix: info popups vulnerability + rainfall forecast AB#18652
</commit_message>
<xml_diff>
--- a/services/API-service/src/scripts/json/layer-popup-info.xlsx
+++ b/services/API-service/src/scripts/json/layer-popup-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\services\API-service\src\scripts\json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6DA600-603A-4932-BA18-3D3834337217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594ED977-9ED9-4C80-88E8-A95646439490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15195" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
+    <workbookView xWindow="13770" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1428,15 +1428,9 @@
 &lt;p&gt;&lt;strong&gt;Population source:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a target='_blank' href="https://www.ciesin.columbia.edu/data/hrsl/"&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>This layer shows a dynamic rainfall probability forecast (updated monthly with the model run). It is visualised in yellow (low) to red (high) gradient on the map. The rainfall map layer indicates the probability for below average rainfall based on SEAS5 seasonal forecasting rainfall data from ECMWF.&lt;br /&gt;&lt;br /&gt;For the legend see &lt;a target='_blank' href='https://www.icpac.net/seasonal-forecast/'&gt;https://www.icpac.net/seasonal-forecast/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt; Source link:  &lt;a target='_blank' href='https://www.ecmwf.int/en/forecasts/datasets'&gt;SEAS5 Seasonal Forecasts&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>This layer represents the locations of the water points. They are visualised as drop pins with a water drop on the map. You can click on each pin drop to find the number and location of the waterpoint. These are the functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Waterpoints source: &lt;a target='_blank' href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;</t>
   </si>
   <si>
-    <t>This layer shows the drought vulnerability index. It is visualised in shades of grey or purple in the map depending on if there's a trigger. The drought vulnerability index is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts of Drought. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female-headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For further information please refer to the EAP.</t>
-  </si>
-  <si>
     <t>This layer represents the locations of the local branches. It is visualised as drop pins with a Red Cross icon. The source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Uganda Red Cross Society (URCS). Year: 2020.</t>
   </si>
   <si>
@@ -1450,6 +1444,12 @@
   </si>
   <si>
     <t>Community notifications are sent via volunteers that have direct contact with the community. They assess the information and fill in the details in a digital form.&lt;br&gt;&lt;br&gt;The notifications are visualized as drop pins with a bell icon on the map.&lt;br&gt;&lt;br&gt;&lt;strong&gt;What to do?&lt;/strong&gt; Click on the drop pin to open it and see the information attached to it. Some notifications contain photos.&lt;br&gt;&lt;br&gt;The pins on the map will stay on the map until manually deleted. Make sure to delete irrelevant and old notifications.&lt;br&gt;&lt;br&gt;&lt;strong&gt;All sent notifications including deleted ones&lt;/strong&gt;: &lt;a href='https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx'&gt;https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>This layer shows the vulnerability index. It is visualised in shades of grey or purple in the map depending on if there's a trigger. The vulnerability index is a copy of the 'flood vulnerabilty index' used in the IBF Floods portal. It is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female-headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For further information please refer to the EAP. For sources of the components, see the source layers in the IBF floods portal.</t>
+  </si>
+  <si>
+    <t>This layer shows a dynamic rainfall probability forecast for the (first) month of the selected timeline button. It is updated monthly with the model run. It is visualised in yellow (low) to red (high) gradient on the map. The rainfall map layer indicates the probability for below average rainfall based on SEAS5 seasonal forecasting rainfall data from ECMWF.&lt;br /&gt;&lt;br /&gt;For the legend see &lt;a target='_blank' href='https://www.icpac.net/seasonal-forecast/'&gt;https://www.icpac.net/seasonal-forecast/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt; Source link:  &lt;a target='_blank' href='https://www.ecmwf.int/en/forecasts/datasets'&gt;SEAS5 Seasonal Forecasts&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -1961,9 +1961,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D31E7F-BFF5-4ADE-901A-4F6BC662C23D}">
   <dimension ref="A1:S429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F166" sqref="F166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2921,7 +2921,7 @@
       <c r="E15" s="21"/>
       <c r="F15" s="5"/>
       <c r="G15" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="str">
@@ -3440,7 +3440,7 @@
         <v>116</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>7</v>
@@ -3451,7 +3451,7 @@
       <c r="E23" s="21"/>
       <c r="F23" s="5"/>
       <c r="G23" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="14" t="str">
@@ -9929,7 +9929,7 @@
       <c r="E118" s="21"/>
       <c r="F118" s="5"/>
       <c r="G118" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H118" s="19"/>
       <c r="I118" s="14" t="str">
@@ -13113,7 +13113,7 @@
         <v>"rainfall_forecast": {"ETH": {"drought": "The rainfall map layer indicates the seasonal forecasting rainfall data for the floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;For the legend see &lt;a target='_blank' href='https://www.icpac.net/seasonal-forecast/'&gt;https://www.icpac.net/seasonal-forecast/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="9" t="s">
         <v>116</v>
       </c>
@@ -13129,7 +13129,7 @@
       <c r="E166" s="21"/>
       <c r="F166" s="5"/>
       <c r="G166" s="6" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="H166" s="19"/>
       <c r="I166" s="14" t="str">
@@ -13150,7 +13150,7 @@
       </c>
       <c r="M166" s="13" t="str">
         <f t="shared" si="37"/>
-        <v>"drought": "This layer shows a dynamic rainfall probability forecast (updated monthly with the model run). It is visualised in yellow (low) to red (high) gradient on the map. The rainfall map layer indicates the probability for below average rainfall based on SEAS5 seasonal forecasting rainfall data from ECMWF.&lt;br /&gt;&lt;br /&gt;For the legend see &lt;a target='_blank' href='https://www.icpac.net/seasonal-forecast/'&gt;https://www.icpac.net/seasonal-forecast/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt; Source link:  &lt;a target='_blank' href='https://www.ecmwf.int/en/forecasts/datasets'&gt;SEAS5 Seasonal Forecasts&lt;/a&gt;"</v>
+        <v>"drought": "This layer shows a dynamic rainfall probability forecast for the (first) month of the selected timeline button. It is updated monthly with the model run. It is visualised in yellow (low) to red (high) gradient on the map. The rainfall map layer indicates the probability for below average rainfall based on SEAS5 seasonal forecasting rainfall data from ECMWF.&lt;br /&gt;&lt;br /&gt;For the legend see &lt;a target='_blank' href='https://www.icpac.net/seasonal-forecast/'&gt;https://www.icpac.net/seasonal-forecast/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt; Source link:  &lt;a target='_blank' href='https://www.ecmwf.int/en/forecasts/datasets'&gt;SEAS5 Seasonal Forecasts&lt;/a&gt;"</v>
       </c>
       <c r="N166" s="26" t="str">
         <f t="shared" si="38"/>
@@ -13174,7 +13174,7 @@
       </c>
       <c r="S166" s="13" t="str">
         <f t="shared" si="43"/>
-        <v>"UGA": {"drought": "This layer shows a dynamic rainfall probability forecast (updated monthly with the model run). It is visualised in yellow (low) to red (high) gradient on the map. The rainfall map layer indicates the probability for below average rainfall based on SEAS5 seasonal forecasting rainfall data from ECMWF.&lt;br /&gt;&lt;br /&gt;For the legend see &lt;a target='_blank' href='https://www.icpac.net/seasonal-forecast/'&gt;https://www.icpac.net/seasonal-forecast/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt; Source link:  &lt;a target='_blank' href='https://www.ecmwf.int/en/forecasts/datasets'&gt;SEAS5 Seasonal Forecasts&lt;/a&gt;"}},</v>
+        <v>"UGA": {"drought": "This layer shows a dynamic rainfall probability forecast for the (first) month of the selected timeline button. It is updated monthly with the model run. It is visualised in yellow (low) to red (high) gradient on the map. The rainfall map layer indicates the probability for below average rainfall based on SEAS5 seasonal forecasting rainfall data from ECMWF.&lt;br /&gt;&lt;br /&gt;For the legend see &lt;a target='_blank' href='https://www.icpac.net/seasonal-forecast/'&gt;https://www.icpac.net/seasonal-forecast/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt; Source link:  &lt;a target='_blank' href='https://www.ecmwf.int/en/forecasts/datasets'&gt;SEAS5 Seasonal Forecasts&lt;/a&gt;"}},</v>
       </c>
     </row>
     <row r="167" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -13993,7 +13993,7 @@
       <c r="E179" s="21"/>
       <c r="F179" s="5"/>
       <c r="G179" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H179" s="7">
         <v>44575</v>
@@ -14125,7 +14125,7 @@
       <c r="E181" s="21"/>
       <c r="F181" s="5"/>
       <c r="G181" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H181" s="19"/>
       <c r="I181" s="14" t="str">
@@ -15237,7 +15237,7 @@
 &lt;p&gt;&lt;strong&gt;Latest updated:&lt;/strong&gt; month, year&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="9" t="s">
         <v>116</v>
       </c>
@@ -15253,7 +15253,7 @@
       <c r="E197" s="21"/>
       <c r="F197" s="5"/>
       <c r="G197" s="6" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="H197" s="19"/>
       <c r="I197" s="14" t="str">
@@ -15274,7 +15274,7 @@
       </c>
       <c r="M197" s="13" t="str">
         <f t="shared" si="48"/>
-        <v>"drought": "This layer shows the drought vulnerability index. It is visualised in shades of grey or purple in the map depending on if there's a trigger. The drought vulnerability index is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts of Drought. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female-headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For further information please refer to the EAP."</v>
+        <v>"drought": "This layer shows the vulnerability index. It is visualised in shades of grey or purple in the map depending on if there's a trigger. The vulnerability index is a copy of the 'flood vulnerabilty index' used in the IBF Floods portal. It is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female-headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For further information please refer to the EAP. For sources of the components, see the source layers in the IBF floods portal."</v>
       </c>
       <c r="N197" s="26" t="str">
         <f t="shared" si="49"/>
@@ -15298,7 +15298,7 @@
       </c>
       <c r="S197" s="13" t="str">
         <f t="shared" si="54"/>
-        <v>"vulnerability_index": {"UGA": {"drought": "This layer shows the drought vulnerability index. It is visualised in shades of grey or purple in the map depending on if there's a trigger. The drought vulnerability index is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts of Drought. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female-headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For further information please refer to the EAP."}},</v>
+        <v>"vulnerability_index": {"UGA": {"drought": "This layer shows the vulnerability index. It is visualised in shades of grey or purple in the map depending on if there's a trigger. The vulnerability index is a copy of the 'flood vulnerabilty index' used in the IBF Floods portal. It is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female-headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For further information please refer to the EAP. For sources of the components, see the source layers in the IBF floods portal."}},</v>
       </c>
     </row>
     <row r="198" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
@@ -16131,7 +16131,7 @@
       <c r="E210" s="21"/>
       <c r="F210" s="5"/>
       <c r="G210" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H210" s="7">
         <v>44659</v>
@@ -16263,7 +16263,7 @@
       <c r="E212" s="21"/>
       <c r="F212" s="5"/>
       <c r="G212" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H212" s="19"/>
       <c r="I212" s="14" t="str">
@@ -28070,7 +28070,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/2cQJi+i8cAZdTOEtvA14sKUkbKkCfiNOt5+1emBF3SA7mHaD944VfbOvqD121Wkbo/0g52ddVMadxgrCkXx0A==" saltValue="3UdpGa7ferffexeCF0WtDA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+WbQO8f8Nx34PYcKJES9TepF4Pm6IvnaJOYJUTrnaSwBT7RqXOi+WZwQyvlh0G1IxPrOU80+gR8dQkR9ighwAA==" saltValue="TFLaLkkRclnmt5Py69a2tg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>

</xml_diff>

<commit_message>
fix: update MWI flash-floods info popups AB#25047
</commit_message>
<xml_diff>
--- a/services/API-service/src/scripts/json/layer-popup-info.xlsx
+++ b/services/API-service/src/scripts/json/layer-popup-info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\services\API-service\src\scripts\json\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\510\IBF-system\services\API-service\src\scripts\json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EE05C2-A53D-4BCC-AAFE-0E35972DFED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A00A673-71E5-419A-BB68-C580F96A2AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13770" yWindow="-16320" windowWidth="29040" windowHeight="15225" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20332" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1262,56 +1262,11 @@
     <t>This layer represents the cropland. It is visualised in yellow on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Cropland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010</t>
   </si>
   <si>
-    <t>This layer shows the buildings in the potentially affected Traditional Authorities. Each building has either a green or a red outline. Green when it is outside the potentially inundated area so safe and red when it is inside the potentially inundated area so in danger.
-Source: Openstreetmap</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This layer shows the buildings in the potentially affected Traditional Authorities. Each building has either a green or a red outline. Green when it is outside the potentially inundated area so safe and red when it is inside the potentially inundated area so in danger.&lt;/p&gt;
-&lt;br&gt;
-&lt;p&gt;Source: Openstreetmap&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>This layer shows the area that is potentially flooding in this event. The fooded area is derived from the HEC-RAS flood model. The model resulted in scenario's that are related to the forecasted rainfall. The rainfall forecast from GFS is every 6 hours matched for each Traditional Authority to the scenario from the flood model.
-The color indicates the depth of the flooded area, yellow means the area is only flooded with a shallow layer of water and red means a deep layer of water, with the different shades of orange somewhere in between.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This layer shows the area that is potentially flooding in this event. The fooded area is derived from the HEC-RAS flood model. The model resulted in scenario's that are related to the forecasted rainfall. The rainfall forecast from GFS is every 6 hours matched for each Traditional Authority to the scenario from the flood model.&lt;/p&gt;
-&lt;p&gt;The color indicates the depth of the flooded area, yellow means the area is only flooded with a shallow layer of water and red means a deep layer of water, with the different shades of orange somewhere in between.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Source: Openstreetmap</t>
-  </si>
-  <si>
-    <t>This indicator shows the total number of buildings in the potentially flooded area. The number is filtered on the selected area (see above).
-Source: Openstreetmap</t>
-  </si>
-  <si>
-    <t>This layer shows the Health Sites in the potentially affected Traditional Authorities. Each Health Site has either a blue or a red marker. Blue when it is outside the potentially inundated area so safe and red when it is inside the potentially inundated area so in danger.
-Source: Cloud2Street</t>
-  </si>
-  <si>
-    <t>This indicator shows the total amount of kilometers of roads in the potentially flooded area. The number is filtered on the selected area (see above). The roads are not filtered on the type of road so it includes more roads than the map layer.
-Source: Openstreetmap</t>
   </si>
   <si>
     <t>This layer shows the roads in the potentially affected Traditional Authorities. Each road is displayed as either a green or a red line. Green when it is outside the potentially inundated area so not exposed and red when it is inside the potentially inundated area so potentially flooded. This layer only shows the main roads which is different from the indicator in the middle column.
 Source: Openstreetmap</t>
-  </si>
-  <si>
-    <t>This indicator shows the total number of health sites in the potentially flooded area. The number is filtered on the selected area (see above).
-Source: Cloud2Street</t>
-  </si>
-  <si>
-    <t>This indicator shows the total number of school buildings in the potentially flooded area. The number is filtered on the selected area (see above).
-Source: Cloud2Street</t>
-  </si>
-  <si>
-    <t>This indicator shows the total number of water points in the potentially flooded area. The number is filtered on the selected area (see above).
-Source: mWater &lt;https://portal.mwater.co/#/&gt;</t>
-  </si>
-  <si>
-    <t>This layer shows the amount of people that is potentially exposed per geographic area. This is calculated by determining the amount of people that live in the potentially flooded area.
-Source: Meta on HDX &lt;https://data.humdata.org/dataset/highresolutionpopulationdensitymaps-mwi&gt;</t>
   </si>
   <si>
     <t>This layer shows the main rivers that are used in the flood model.
@@ -1337,60 +1292,103 @@
 &lt;p&gt;Source: Openstreetmap&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;This layer shows the amount of people that is potentially exposed per geographic area. This is calculated by determining the amount of people that live in the potentially flooded area.&lt;/p&gt;
+    <t>&lt;p&gt;Number of people exposed is calculated by the population living in the flood extent area within the administrative areas currently triggered. The number of people and the flood extent are derived from the below sources.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;    &lt;li&gt;Source (Population Data): peanutButter: An R package to produce rapid-response gridded population estimates from building footprints, version 1.0.0 version 1.0.0. Accessed 15-08-2022. WorldPop, University of Southampton. 2021. &amp;nbsp;&lt;a target='_blank' href='https://apps.worldpop.org/peanutButter/'&gt;https://apps.worldpop.org/peanutButter/&lt;/a&gt;&lt;/li&gt;    &lt;li&gt;Source Flood Extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Number of people exposed is calculated by the population living in the flood extent area within the manucipality currently triggered. The number of people and the flood extent are derived from the below sources.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Source (Population Data): High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Source Flood Extent: The flood extent maps are generated by the National Operational Assesment of Hazards(NOAH) project.&lt;a target='_blank' href='https://noah.up.edu.ph/'&gt;https://noah.up.edu.ph/&lt;/a&gt; The 25-year rain return flood hazard maps show low, medium, and high flood hazards represented as yellow, orange, and red respectively. Flood hazards consider take both the height and velocity of the water into consideration and calculates the hazard levels based on the danger they pose to people and structures. Generally, for an average Filipino with a height of 5’ 6”, areas with flood depths from the knee down can be considered to have low hazard levels. Those with flood depths ranging from the knee to neck are considered to have medium hazard levels, and those covered with floods that are higher than the neck have high hazard levels. However, since the flow velocity is also considered, areas that have shallow but fast-flowing flood waters may have a higher hazard level than that denoted by the height of the flood covering it.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 10-years) based on a global hydrological model.&lt;br&gt;&lt;br&gt;Source link: Flood hazard map of the World - 10-year return period. European Commission, Joint Research Centre (JRC). 2016. &lt;a target='_blank' href='https://data.jrc.ec.europa.eu/dataset/jrc-floods-floodmapgl_rp10y-tif'&gt;Flood hazard map of the World - 10-year return period - European Commission (europa.eu)&lt;/a&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>gauges</t>
+  </si>
+  <si>
+    <t>The river gauge layer shows you the location of river gauges on the map, they are visualised as blue drop pins with a river icon. Clicking on a drop pin opens a pop up containing information about the current water level in meters above sea level (mMSL) this is measured daily with the latest model run. The difference compared to 24 hours ago is shown in green for decrease or red for increase. The reference water level is the typical level for this station during this season.</t>
+  </si>
+  <si>
+    <t>This layer displays the buildings within Traditional Authorities that may be affected. Each building is outlined in either green or red. Green indicates it is outside the potentially inundated area and safe. Red indicates it is inside the potentially inundated area and at risk.
+Source: Openstreetmap</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This layer displays the buildings within Traditional Authorities that may be affected. Each building is outlined in either green or red. Green indicates it is outside the potentially inundated area and safe. Red indicates it is inside the potentially inundated area and at risk.&lt;/p&gt;
+&lt;br&gt;
+&lt;p&gt;Source: Openstreetmap&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>This indicator estimates potential economic damage based on global depth-damage functions provided by the JRC (refer to the publication at https://op.europa.eu/en/publication-detail/-/publication/a20ecfa5-200e-11e7-84e2-01aa75ed71a1/language-en). The assessment differentiates damage according to water depth and land use, specifically utilizing the land use classes of urban and agricultural from the ESA WorldCover 2020 dataset (refer to the website https://worldcover2020.esa.int/). The monetary value is converted from Euro to Malawi Kwacha using a fixed exchange rate of xx.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This indicator estimates potential economic damage based on global depth-damage functions provided by the JRC (refer to the publication at &lt;a target="_blank" hfref="https://op.europa.eu/en/publication-detail/-/publication/a20ecfa5-200e-11e7-84e2-01aa75ed71a1/language-en"&gt;https://op.europa.eu/en/publication-detail/-/publication/a20ecfa5-200e-11e7-84e2-01aa75ed71a1/language-en&lt;/a&gt;). The assessment differentiates damage according to water depth and land use, specifically utilizing the land use classes of urban and agricultural from the ESA WorldCover 2020 dataset (refer to the website &lt;a target="_blank" href="https://worldcover2020.esa.int/"&gt;https://worldcover2020.esa.int/&lt;/a&gt;). The monetary value is converted from Euro to Malawi Kwacha using a fixed exchange rate of xx.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>This layer shows the potentially flooded area in the current event, determined by the HEC-RAS flood model. The model produces scenarios correlated with forecasted rainfall. GFS rainfall forecasts, updated every 6 hours, are synchronized with the flood model scenarios for each Traditional Authority. The color scheme represents the depth of the flooded area: yellow signifies a shallow layer of water, red signifies a deep layer, and various shades of orange signifies intermediate depths.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This layer shows the potentially flooded area in the current event, determined by the HEC-RAS flood model. The model produces scenarios correlated with forecasted rainfall. GFS rainfall forecasts, updated every 6 hours, are synchronized with the flood model scenarios for each Traditional Authority.&lt;/p&gt;&lt;p&gt;The color scheme represents the depth of the flooded area: yellow signifies a shallow layer of water, red signifies a deep layer, and various shades of orange signifies intermediate depths.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>This layer shows Health Sites within Traditional Authorities that may be affected. Each Health Site is marked with either a blue or red indicator. Blue indicates it is outside the potentially inundated area and safe. Red indicates it is inside the potentially inundated area and at risk.
+Source: Cloud2Street</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This layer shows Health Sites within Traditional Authorities that may be affected. Each Health Site is marked with either a blue or red indicator. Blue indicates it is outside the potentially inundated area and safe. Red indicates it is inside the potentially inundated area and at risk.&lt;/p&gt;
+&lt;br&gt;
+&lt;p&gt;Source: Cloud2Street&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>This indicator shows the total number of buildings within the potentially flooded area, filtered based on the selected area (see above).
+Source: Openstreetmap</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This indicator shows the total number of buildings within the potentially flooded area, filtered based on the selected area (see above).&lt;/p&gt;
+&lt;br&gt;
+&lt;p&gt;Source: Openstreetmap&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>This indicator shows the total number of health sites in the potentially flooded area, Filtered based on the selected area (see above).
+Source: Cloud2Street</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This indicator shows the total number of health sites in the potentially flooded area, Filtered based on the selected area (see above).&lt;/p&gt;
+&lt;br&gt;
+&lt;p&gt;Source: Cloud2Street&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>This indicator shows the total amount of kilometers of roads in the potentially flooded area, Filtered based on the selected area (see above). The roads are not filtered by the type of road so it includes more roads than is shown in the map layer.
+Source: Openstreetmap</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This indicator shows the total amount of kilometers of roads in the potentially flooded area, Filtered based on the selected area (see above). The roads are not filtered by the type of road so it includes more roads than is shown in the map layer.&lt;/p&gt;
+&lt;br&gt;
+&lt;p&gt;Source: Openstreetmap&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>This indicator shows the total number of school buildings in the potentially flooded area, Filtered based on the selected area (see above).
+Source: Cloud2Street</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This indicator shows the total number of school buildings in the potentially flooded area, Filtered based on the selected area (see above).&lt;/p&gt;
+&lt;br&gt;
+&lt;p&gt;Source: Cloud2Street&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>This indicator shows the total number of water points in the potentially flooded area, Filtered based on the selected area (see above).
+Source: mWater &lt;https://portal.mwater.co/#/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This indicator shows the total number of water points in the potentially flooded area, Filtered based on the selected area (see above).&lt;/p&gt;
+&lt;br&gt;
+&lt;p&gt;Source: &lt;a target='_blank' href="https://portal.mwater.co/#/"&gt;mWater &lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>This layer shows the amount of people that is potentially exposed per geographic area. This is calculated by determining the amount of people who live in the potentially flooded area.
+Source: Meta on HDX &lt;https://data.humdata.org/dataset/highresolutionpopulationdensitymaps-mwi&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This layer shows the amount of people that is potentially exposed per geographic area. This is calculated by determining the amount of people who live in the potentially flooded area.&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: &lt;a target='_blank' href="https://data.humdata.org/dataset/highresolutionpopulationdensitymaps-mwi"&gt;Meta on HDX &lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This indicator shows the total number of water points in the potentially flooded area. The number is filtered on the selected area (see above).&lt;/p&gt;
-&lt;br&gt;
-&lt;p&gt;Source: &lt;a target='_blank' href="https://portal.mwater.co/#/"&gt;mWater &lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This indicator shows the total number of school buildings in the potentially flooded area. The number is filtered on the selected area (see above).&lt;/p&gt;
-&lt;br&gt;
-&lt;p&gt;Source: Cloud2Street&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This indicator shows the total amount of kilometers of roads in the potentially flooded area. The number is filtered on the selected area (see above). The roads are not filtered on the type of road so it includes more roads than the map layer.&lt;/p&gt;
-&lt;br&gt;
-&lt;p&gt;Source: Openstreetmap&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This indicator shows the total number of health sites in the potentially flooded area. The number is filtered on the selected area (see above).&lt;/p&gt;
-&lt;br&gt;
-&lt;p&gt;Source: Cloud2Street&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This indicator shows the total number of buildings in the potentially flooded area. The number is filtered on the selected area (see above).&lt;/p&gt;
-&lt;br&gt;
-&lt;p&gt;Source: Openstreetmap&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This layer shows the Health Sites in the potentially affected Traditional Authorities. Each Health Site has either a blue or a red marker. Blue when it is outside the potentially inundated area so safe and red when it is inside the potentially inundated area so in danger.&lt;/p&gt;
-&lt;br&gt;
-&lt;p&gt;Source: Cloud2Street&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>This indicator shows the estimated potential economic damage. It is based on global depth-damage functions from the jrc (see publication &lt;https://op.europa.eu/en/publication-detail/-/publication/a20ecfa5-200e-11e7-84e2-01aa75ed71a1/language-en&gt;). It distinguishes the damage by water depth and land use, the land use classes urban and agricultural are used, based on the ESA WorldCover 2020 dataset (see website &lt;https://worldcover2020.esa.int/&gt;). The value is converted from Euro to Malawi Kwacha with a fixed exchange rate of xx.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This indicator shows the estimated potential economic damage. It is based on global depth-damage functions from the jrc (see &lt;a target='_blank' href="https://op.europa.eu/en/publication-detail/-/publication/a20ecfa5-200e-11e7-84e2-01aa75ed71a1/language-en"&gt;publication&lt;/a&gt;). It distinguishes the damage by water depth and land use, the land use classes urban and agricultural are used, based on the ESA WorldCover 2020 dataset (see &lt;a target='_blank' href="https://worldcover2020.esa.int/"&gt;website&lt;/a&gt;). The value is converted from Euro to Malawi Kwacha with a fixed exchange rate of xx.</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Number of people exposed is calculated by the population living in the flood extent area within the administrative areas currently triggered. The number of people and the flood extent are derived from the below sources.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;    &lt;li&gt;Source (Population Data): peanutButter: An R package to produce rapid-response gridded population estimates from building footprints, version 1.0.0 version 1.0.0. Accessed 15-08-2022. WorldPop, University of Southampton. 2021. &amp;nbsp;&lt;a target='_blank' href='https://apps.worldpop.org/peanutButter/'&gt;https://apps.worldpop.org/peanutButter/&lt;/a&gt;&lt;/li&gt;    &lt;li&gt;Source Flood Extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Number of people exposed is calculated by the population living in the flood extent area within the manucipality currently triggered. The number of people and the flood extent are derived from the below sources.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Source (Population Data): High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Source Flood Extent: The flood extent maps are generated by the National Operational Assesment of Hazards(NOAH) project.&lt;a target='_blank' href='https://noah.up.edu.ph/'&gt;https://noah.up.edu.ph/&lt;/a&gt; The 25-year rain return flood hazard maps show low, medium, and high flood hazards represented as yellow, orange, and red respectively. Flood hazards consider take both the height and velocity of the water into consideration and calculates the hazard levels based on the danger they pose to people and structures. Generally, for an average Filipino with a height of 5’ 6”, areas with flood depths from the knee down can be considered to have low hazard levels. Those with flood depths ranging from the knee to neck are considered to have medium hazard levels, and those covered with floods that are higher than the neck have high hazard levels. However, since the flow velocity is also considered, areas that have shallow but fast-flowing flood waters may have a higher hazard level than that denoted by the height of the flood covering it.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 10-years) based on a global hydrological model.&lt;br&gt;&lt;br&gt;Source link: Flood hazard map of the World - 10-year return period. European Commission, Joint Research Centre (JRC). 2016. &lt;a target='_blank' href='https://data.jrc.ec.europa.eu/dataset/jrc-floods-floodmapgl_rp10y-tif'&gt;Flood hazard map of the World - 10-year return period - European Commission (europa.eu)&lt;/a&gt;.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>gauges</t>
-  </si>
-  <si>
-    <t>The river gauge layer shows you the location of river gauges on the map, they are visualised as blue drop pins with a river icon. Clicking on a drop pin opens a pop up containing information about the current water level in meters above sea level (mMSL) this is measured daily with the latest model run. The difference compared to 24 hours ago is shown in green for decrease or red for increase. The reference water level is the typical level for this station during this season.</t>
   </si>
 </sst>
 </file>
@@ -1599,9 +1597,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1639,7 +1637,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1745,7 +1743,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1887,7 +1885,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1898,29 +1896,29 @@
   <dimension ref="A1:S419"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E56" sqref="E56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.3125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1015625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.5234375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="57.5234375" style="21" customWidth="1"/>
+    <col min="1" max="1" width="18.3046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.07421875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.53515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="57.53515625" style="21" customWidth="1"/>
     <col min="6" max="6" width="17" style="15" customWidth="1"/>
     <col min="7" max="7" width="102" style="16" customWidth="1"/>
     <col min="8" max="8" width="14" style="17" customWidth="1"/>
     <col min="9" max="9" width="11" style="14" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.3125" style="14" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.3046875" style="14" hidden="1" customWidth="1"/>
     <col min="11" max="12" width="22" style="14" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="35.1015625" style="12" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="35.1015625" style="25" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="35.07421875" style="12" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="35.07421875" style="25" hidden="1" customWidth="1"/>
     <col min="15" max="19" width="9" style="14" hidden="1" customWidth="1"/>
-    <col min="110" max="110" width="93.1015625" customWidth="1"/>
+    <col min="110" max="110" width="93.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1955,7 +1953,7 @@
       <c r="R1" s="12"/>
       <c r="S1" s="12"/>
     </row>
-    <row r="2" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>99</v>
       </c>
@@ -2023,7 +2021,7 @@
         <v>{"layers-section": {"affected_population": {"PHL": {"typhoon": "&lt;p&gt;The number of people affected is calculated based on the predicted number of completely damaged houses, which is derived from the typhoon impact predicting model. To derive a methodology to estimate the number of affected people from a predicted number of completely damaged houses, we performed a log fit between the number of completely damaged houses and the number of affected people for past typhoon events using data derived from DROMIC reports. To estimate potential number of affected population this formula is applied to the predicted number of damaged houses. &lt;p&gt; "}},</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A3" s="8" t="s">
         <v>99</v>
       </c>
@@ -2087,7 +2085,7 @@
         <v>"alert_threshold": {"EGY": {"heavy-rain": "Egyptian RCS can respond accordingly to their EAP/ SOP when the rainfall forecast from Global Forecast System for the lead times of 3- or 5- or 7 days exceeds the defined thresholds, which will be anticipated to occur in some regions of Egypt. The defined threshold corresponds to a 5-year return period heavy rainfall event."},</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A4" s="8" t="s">
         <v>99</v>
       </c>
@@ -2151,7 +2149,7 @@
         <v>"ETH": {"drought": "Rainfall forecast based on NMA/ICPAC will be used as the primary trigger mechanism before the start of the season. This trigger will provide information with a lead time of up to 1 months. The trigger values for this trigger are for more than 50% of the geographical area of a zone(Admin level 2) a Drier than normal conditions(SPI3&lt; -1) are predicted based on the 1 month Standard precipitation index (SPI3). The SPI3 values will be based on seasonal rainfall forecast issued by NMA/ICPAC. In addition to the above requirement the probability of below normal rain should be at 45% based on probabilistic forecast information provided by NMA/ICPAC.",</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
         <v>99</v>
       </c>
@@ -2215,7 +2213,7 @@
         <v>"floods": "The ERCS will act based on the developed trigger table when the Global Floods awareness system forecast indicates a level of river discharge greater or equal to a level of 10 years return period with a probability of at least 75% forecast uncertainty within 7 days lead time period.",</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A6" s="8" t="s">
         <v>99</v>
       </c>
@@ -2281,7 +2279,7 @@
         <v>"malaria": "An alert is released when two conditions are simultaneously the relative number of malaria cases is anomalous accordance to WHO guidelines, by comparing it to its monthly averages, the second condition is that the absolute number of malaria cases is high and thus likely to require humanitarian intervention."},</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:19" ht="204" x14ac:dyDescent="0.4">
       <c r="A7" s="8" t="s">
         <v>99</v>
       </c>
@@ -2357,7 +2355,7 @@
 &lt;p&gt;For further information please refer to the EAP&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:19" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A8" s="8" t="s">
         <v>99</v>
       </c>
@@ -2433,7 +2431,7 @@
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
         <v>99</v>
       </c>
@@ -2497,7 +2495,7 @@
         <v>"MWI": {"flash-floods": "Not currently available",</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:19" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A10" s="8" t="s">
         <v>99</v>
       </c>
@@ -2573,7 +2571,7 @@
 &lt;p&gt;Latest updated: August 2022&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:19" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A11" s="8" t="s">
         <v>99</v>
       </c>
@@ -2639,7 +2637,7 @@
         <v>"PHL": {"dengue": "Administrative divisions that reached alert threshold, in terms of number of potential cases. &lt;br /&gt;&lt;br /&gt; See definition at: &lt;a target='_blank' href='https://rodekruis.sharepoint.com/sites/510-CRAVK-510/Gedeelde%20%20documenten/Forms/AllItems.aspx?id=%2Fsites%2F510%2DCRAVK%2D510%2FGedeelde%20%20documenten%2F%5BRD%5D%20Epidemics%20Priority%20Index%2FIBF%2Ddengue%2Fdocuments%2FIBF%5Fdengue%5Ftechnical%5Fnote%2Epdf&amp;parent=%2Fsites%2F510%2DCRAVK%2D510%2FGedeelde%20%20documenten%2F%5BRD%5D%20Epidemics%20Priority%20Index%2FIBF%2Ddengue%2Fdocuments&amp;p=true&amp;originalPath=aHR0cHM6Ly9yb2Rla3J1aXMuc2hhcmVwb2ludC5jb20vc2l0ZXMvNTEwLUNSQVZLLTUxMC9fbGF5b3V0cy8xNS9ndWVzdGFjY2Vzcy5hc3B4P2RvY2lkPTBmOTI0OWIzNWRhNGQ0YzBhOTg1YjMzMzkzZmMzODhkZiZhdXRoa2V5PUFRU0xubmFmR0YtTTJ0MUNHSWcwaGRBJmV4cGlyYXRpb249MjAyMi0wNi0xNFQyMiUzYTAwJTNhMDAuMDAwWiZydGltZT1TS016R0dzeDJVZw'&gt; link to technical documentation&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A12" s="8" t="s">
         <v>99</v>
       </c>
@@ -2705,7 +2703,7 @@
         <v>"floods": "&lt;p&gt;The layer shows each county triggered based on two parameters from the 3-days GLOFAS forecast on a daily basis: the return period of the forecasted flood and the probability of occurrence. The trigger will activate when GloFAS issues a forecast of at least 50% probability of occurrence of a 5 year return period flood within the next 7 days. The GLOFAS flood forecast triggers except in the  manucipalities where the False Alarm Ratio (RAR) &amp;gt;0.5&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Source link&lt;/strong&gt;: &lt;a target='_blank' href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Latest updated:&amp;nbsp;&lt;/strong&gt;September 2021&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A13" s="8" t="s">
         <v>99</v>
       </c>
@@ -2771,7 +2769,7 @@
         <v>"typhoon": "&lt;p&gt;The predicted impact (72 hours before landfall) is more than 10% of houses being totally damaged at municipal level, in at least 3 municipalities. The source for predicted impact is 510 typhoon impact prediction model.&lt;br&gt;&lt;br&gt;Only municipalities that are included in the EAP can reach a triggered state. For other municipalities all data - such as predicted impact - is visible in the map, but they will never turn in to a triggered state.&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:19" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A14" s="8" t="s">
         <v>99</v>
       </c>
@@ -2841,7 +2839,7 @@
 &lt;strong&gt;Latest updated:&amp;nbsp;&lt;/strong&gt;September 2021"},</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A15" s="8" t="s">
         <v>99</v>
       </c>
@@ -2905,7 +2903,7 @@
         <v>"UGA": {"drought": "&lt;P&gt;This layer represents the areas in which the trigger threshold has been reached. It is visualised on the map as red outlines around the exposed areas. &lt;br&gt; The primary trigger mechanism uses rainfall forecasts based on ECMWF before the start of the season. This trigger will provide information with a lead time of up to 3 months. The trigger values for this trigger are for more than 30% of the geographical area of a district (admin level 2) predicting drier than normal (below average rainfall) conditions. The rainfall values are based on the seasonal rainfall forecast issued by ECMWF. The probability of below normal rain should be at least 45% based on probabilistic forecast information provided by ECMWF.&lt;/P&gt;",</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:19" ht="77.150000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="8" t="s">
         <v>99</v>
       </c>
@@ -2969,7 +2967,7 @@
         <v>"floods": "URCS will activate this EAP when GloFAS issues a forecast of at least &lt;b&gt;60% probability&lt;/b&gt; (based on the different ensemble runs) &lt;b&gt;of a 5-year return period&lt;/b&gt; flood occurring in flood prone districts, which will be anticipated to affect &lt;b&gt;more than 1,000hh&lt;/b&gt;. The EAP will be triggered with a &lt;b&gt;lead time of 7 days&lt;/b&gt; and a FAR of &lt;b&gt;not more than 0.5.&lt;/b&gt;",</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
         <v>99</v>
       </c>
@@ -3037,7 +3035,7 @@
         <v>"heavy-rain": "&lt;p&gt;The alert threshold shows which administrative areas are expecting a large amount of rainfall, exceeding a defined threshold (60 mm).&lt;/p&gt;&lt;p&gt;You can find information about the rainfall forecast in the Rainfall Extent layer.&lt;/p&gt;&lt;p&gt;The defined 1-day cumulative threshold is estimated based on rainfall data collected over a period of 2 years and is provided by &lt;a target='_blank' href='https://scg.zednet.co.za/'&gt;https://scg.zednet.co.za/&lt;/a&gt;. &lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A18" s="8" t="s">
         <v>99</v>
       </c>
@@ -3101,7 +3099,7 @@
         <v>"ZMB": {"drought": "Not currently available",</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A19" s="8" t="s">
         <v>99</v>
       </c>
@@ -3165,7 +3163,7 @@
         <v>"floods": "The trigger is activated if the daily issued GLOFAS forecast reports a water discharge that exceeds the threshold corresponding to a 10y return period flood in one or more GLOFAS stations. The EAP will be triggered with a lead time of 7 days."},</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:19" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A20" s="8" t="s">
         <v>99</v>
       </c>
@@ -3235,7 +3233,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;The layer shows each province in the country with a drought risk at the end of the growing season (April), and as such determine which provinces are triggered when at least one of their districts is expected to face a +/- 6 year return period drought.&lt;/p&gt; &lt;p&gt;The drought model is to assess a drought prediction skill of the 3-month running average Ni&amp;ntilde;o 3.4 values and initiates a drought risk when there is a potential negative crop yield anomaly predicted. The model is developed based on the XGBoost algorithm tested and trained with historical ENSO: Seasonal ERSSTv5 and CHIRPS Rainfall data in relation to historical negative crop yield anomalies in April, which is used as drought impact proxy. Loss of crops, livestock loss, and child malnutrition and stunting are indicated by the ZRCS DRM working group and representatives from IFRC, PNS, and Red Cross Climate Centre (RCCC) &amp;nbsp;as targeted drought impact&lt;/p&gt;&lt;p&gt;Source links:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Ni&amp;ntilde;o 3.4 (5oNorth-5oSouth) (170-120oWest)) &lt;a target='_blank' href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt&lt;/a&gt;&lt;/li&gt;&lt;li&gt;CHIRPS: Rainfall Estimates from Rain Gauge and Satellite Observations | Climate Hazards Center - UC Santa Barbara (&lt;a target='_blank' href='https://www.chc.ucsb.edu/data/chirps'&gt;https://www.chc.ucsb.edu/data/chirps&lt;/a&gt;)&amp;nbsp;&lt;/li&gt;     &lt;li&gt;Crop Yield data: Izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a target='_blank' href='https://doi.org/10.1594/PANGAEA.909132'&gt;https://doi.org/10.1594/PANGAEA.909132&lt;/a&gt;,Supplement to Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981&amp;ndash;2016. Scientific Data, 7(1), &lt;a target='_blank' href='https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;&lt;/li&gt; &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="103.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:19" ht="103.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="8" t="s">
         <v>99</v>
       </c>
@@ -3249,13 +3247,13 @@
         <v>292</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
       <c r="F21" s="22">
-        <v>45191</v>
+        <v>45281</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>329</v>
+        <v>341</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="13" t="str">
@@ -3276,7 +3274,7 @@
       </c>
       <c r="M21" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>"flash-floods": "&lt;p&gt;This layer shows the buildings in the potentially affected Traditional Authorities. Each building has either a green or a red outline. Green when it is outside the potentially inundated area so safe and red when it is inside the potentially inundated area so in danger.&lt;/p&gt;
+        <v>"flash-floods": "&lt;p&gt;This layer displays the buildings within Traditional Authorities that may be affected. Each building is outlined in either green or red. Green indicates it is outside the potentially inundated area and safe. Red indicates it is inside the potentially inundated area and at risk.&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: Openstreetmap&lt;/p&gt;"</v>
       </c>
@@ -3302,12 +3300,12 @@
       </c>
       <c r="S21" s="12" t="str">
         <f t="shared" si="10"/>
-        <v>"buildings": {"MWI": {"flash-floods": "&lt;p&gt;This layer shows the buildings in the potentially affected Traditional Authorities. Each building has either a green or a red outline. Green when it is outside the potentially inundated area so safe and red when it is inside the potentially inundated area so in danger.&lt;/p&gt;
+        <v>"buildings": {"MWI": {"flash-floods": "&lt;p&gt;This layer displays the buildings within Traditional Authorities that may be affected. Each building is outlined in either green or red. Green indicates it is outside the potentially inundated area and safe. Red indicates it is inside the potentially inundated area and at risk.&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: Openstreetmap&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:19" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A22" s="8" t="s">
         <v>99</v>
       </c>
@@ -3377,7 +3375,7 @@
         <v>"cattle": {"ZWE": {"drought": "&lt;p&gt;Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 &amp;nbsp;as reference unit to aggregate livestock from various species, which is the grazing equivalent of one adult dairy cow producing 3000 kg of milk annually, without additional concentrated foodstuffs.&lt;/p&gt; &lt;p&gt;Source Links :&lt;/p&gt; &lt;ul&gt;     &lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021.&lt;/li&gt;     &lt;li&gt;Source assessment:&lt;br&gt;&lt;a target='_blank' data-fr-linked='true' href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;&lt;/li&gt;     &lt;li&gt;Source Livestock unit (LSU) &lt;a target='_blank' href='https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)'&gt;&amp;nbsp;https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)&lt;/a&gt;&lt;/li&gt; &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:19" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A23" s="8" t="s">
         <v>99</v>
       </c>
@@ -3447,7 +3445,7 @@
         <v>"cattle_exposed": {"ZWE": {"drought": "&lt;p&gt;Number of exposed cattle is calculated by the cattle per province within the droughts alert threshold reached area currently triggered. Livestock numbers cattle exists of the number of cattle multiplied with the Livestock unit (LSU): 1.0 as reference unit, which is the grazing equivalent of one adult dairy cow producing 3000 kg of milk annually, without additional concentrated foodstuffs.&amp;nbsp;&lt;/p&gt;&lt;p&gt;Source Links :&lt;/p&gt; &lt;ul&gt;     &lt;li&gt;Number of cattle mentioned within the 2nd round crop- and livestock assessment report 2020/2021 season. Published: 21st of April 2021.&lt;/li&gt;     &lt;li&gt;Source assessment:&lt;br&gt;&lt;a target='_blank' data-fr-linked='true' href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;&lt;/li&gt;     &lt;li&gt;Source Livestock unit (LSU) &lt;a target='_blank' href='https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)'&gt;&amp;nbsp;https://ec.europa.eu/eurostat/statistics-explained/index.php?title=Glossary:Livestock_unit_(LSU)&lt;/a&gt;&lt;/li&gt; &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:19" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A24" s="8" t="s">
         <v>99</v>
       </c>
@@ -3511,7 +3509,7 @@
         <v>"community_notifications": {"UGA": {"heavy-rain": "Community notifications are sent via volunteers that have direct contact with the community. They assess the information and fill in the details in a digital form.&lt;br&gt;&lt;br&gt;The notifications are visualized as drop pins with a bell icon on the map.&lt;br&gt;&lt;br&gt;&lt;strong&gt;What to do?&lt;/strong&gt; Click on the drop pin to open it and see the information attached to it. Some notifications contain photos.&lt;br&gt;&lt;br&gt;The pins on the map will stay on the map until manually deleted. Make sure to delete irrelevant and old notifications.&lt;br&gt;&lt;br&gt;&lt;strong&gt;All sent notifications including deleted ones&lt;/strong&gt;: &lt;a href='https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx'&gt;https://kobonew.ifrc.org/api/v2/assets/aRa2musHL2hAxERkDHHLmi/export-settings/esL8MBFTLa6RS5XXNbdHcnN/data.xlsx&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:19" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A25" s="8" t="s">
         <v>99</v>
       </c>
@@ -3575,7 +3573,7 @@
         <v>"covid_risk": {"UGA": {"floods": "The COVID-19 Risk Index is a composite index for the context of exposure, vulnerability to COVID and the capacity to anticipate, cope with and recover from the impacts of COVID-19 (a higher percentage indicates a higher risk to COVID-19). The National Society  selected the following criteria below:&lt;br /&gt;&lt;br /&gt;Exposure&lt;ul&gt;&lt;li&gt;population / km2&lt;/li&gt;&lt;/ul&gt;Vulnerability&lt;ul&gt;&lt;li&gt;% population 65+&lt;/li&gt;&lt;li&gt;% poverty incidence&lt;/li&gt;&lt;/ul&gt;Lack of Coping Capacity&lt;ul&gt;&lt;li&gt;% with no toilet facility&lt;/li&gt;&lt;li&gt;% access to safe drinking water&lt;/li&gt;&lt;li&gt;% illiterate&lt;/li&gt;&lt;li&gt;% with mobile access&lt;/li&gt;&lt;li&gt;% with internet access&lt;/li&gt;&lt;li&gt;% received remittances&lt;/li&gt;&lt;li&gt;HIV: incidence per 100&lt;/li&gt;&lt;li&gt;MALARIA: Plasmodium Falciparum incidence per 1000&lt;/li&gt;&lt;li&gt;% households which consume less than two meals per day&lt;/li&gt;&lt;li&gt;# healh facilities per person&lt;/li&gt;&lt;li&gt;% with a health facility within 5 km&lt;/li&gt;&lt;/ul&gt;&lt;br/&gt;Source link: &lt;a target='_blank' href='https://nlrc.maps.arcgis.com/apps/opsdashboard/index.html#/9ca9f0f452b04046b8594a74c31f0c3b'&gt;https://nlrc.maps.arcgis.com/apps/opsdashboard/index.html#/9ca9f0f452b04046b8594a74c31f0c3b&lt;/a&gt;."}},</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A26" s="8" t="s">
         <v>99</v>
       </c>
@@ -3639,7 +3637,7 @@
         <v>"cropland": {"ETH": {"drought": "This layer represents the cropland. It is visualised in yellow on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Cropland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010",</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A27" s="8" t="s">
         <v>99</v>
       </c>
@@ -3703,7 +3701,7 @@
         <v>"floods": "This layer represents the cropland. It is visualised in yellow on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Cropland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:19" ht="233.15" x14ac:dyDescent="0.4">
       <c r="A28" s="8" t="s">
         <v>99</v>
       </c>
@@ -3773,7 +3771,7 @@
         <v>"KEN": {"floods": "This layer represents the cropland. It is visualised in yellow on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Cropland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A29" s="8" t="s">
         <v>99</v>
       </c>
@@ -3837,7 +3835,7 @@
         <v>"UGA": {"drought": "This layer represents the cropland. It is visualised in yellow on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Cropland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010",</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A30" s="8" t="s">
         <v>99</v>
       </c>
@@ -3903,7 +3901,7 @@
         <v>"floods": "This layer represents the cropland. It is visualised in yellow on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Cropland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A31" s="8" t="s">
         <v>99</v>
       </c>
@@ -3967,7 +3965,7 @@
         <v>"ZMB": {"drought": "This layer represents the cropland. It is visualised in yellow on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Cropland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010",</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A32" s="8" t="s">
         <v>99</v>
       </c>
@@ -4031,7 +4029,7 @@
         <v>"floods": "This layer represents the cropland. It is visualised in yellow on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Cropland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:19" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A33" s="8" t="s">
         <v>99</v>
       </c>
@@ -4101,7 +4099,7 @@
         <v>"ZWE": {"drought": "This layer represents the cropland. It is visualised in yellow on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined cropland: consists of 3 land use types&lt;ol&gt;&lt;li&gt;rainfed cropland&lt;/li&gt;&lt;li&gt;mosaic cropland - 50-70% cropland &amp; 20-50% vegetation (grassland/shrubland/forest)&lt;/li&gt;&lt;li&gt;mosaic vegetation - 50-70% vegetation (grassland/shrubland/forest) &amp; 20-50% cropland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Cropland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"}},</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:19" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A34" s="8" t="s">
         <v>99</v>
       </c>
@@ -4115,13 +4113,13 @@
         <v>292</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="F34" s="22">
-        <v>45191</v>
+        <v>45281</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="H34" s="18"/>
       <c r="I34" s="13" t="str">
@@ -4142,7 +4140,7 @@
       </c>
       <c r="M34" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>"flash-floods": "&lt;p&gt;This indicator shows the estimated potential economic damage. It is based on global depth-damage functions from the jrc (see &lt;a target='_blank' href='https://op.europa.eu/en/publication-detail/-/publication/a20ecfa5-200e-11e7-84e2-01aa75ed71a1/language-en'&gt;publication&lt;/a&gt;). It distinguishes the damage by water depth and land use, the land use classes urban and agricultural are used, based on the ESA WorldCover 2020 dataset (see &lt;a target='_blank' href='https://worldcover2020.esa.int/'&gt;website&lt;/a&gt;). The value is converted from Euro to Malawi Kwacha with a fixed exchange rate of xx."</v>
+        <v>"flash-floods": "&lt;p&gt;This indicator estimates potential economic damage based on global depth-damage functions provided by the JRC (refer to the publication at &lt;a target='_blank' hfref='https://op.europa.eu/en/publication-detail/-/publication/a20ecfa5-200e-11e7-84e2-01aa75ed71a1/language-en'&gt;https://op.europa.eu/en/publication-detail/-/publication/a20ecfa5-200e-11e7-84e2-01aa75ed71a1/language-en&lt;/a&gt;). The assessment differentiates damage according to water depth and land use, specifically utilizing the land use classes of urban and agricultural from the ESA WorldCover 2020 dataset (refer to the website &lt;a target='_blank' href='https://worldcover2020.esa.int/'&gt;https://worldcover2020.esa.int/&lt;/a&gt;). The monetary value is converted from Euro to Malawi Kwacha using a fixed exchange rate of xx.&lt;/p&gt;"</v>
       </c>
       <c r="N34" s="25" t="str">
         <f t="shared" si="5"/>
@@ -4166,10 +4164,10 @@
       </c>
       <c r="S34" s="12" t="str">
         <f t="shared" si="10"/>
-        <v>"damage_estimation": {"MWI": {"flash-floods": "&lt;p&gt;This indicator shows the estimated potential economic damage. It is based on global depth-damage functions from the jrc (see &lt;a target='_blank' href='https://op.europa.eu/en/publication-detail/-/publication/a20ecfa5-200e-11e7-84e2-01aa75ed71a1/language-en'&gt;publication&lt;/a&gt;). It distinguishes the damage by water depth and land use, the land use classes urban and agricultural are used, based on the ESA WorldCover 2020 dataset (see &lt;a target='_blank' href='https://worldcover2020.esa.int/'&gt;website&lt;/a&gt;). The value is converted from Euro to Malawi Kwacha with a fixed exchange rate of xx."}},</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+        <v>"damage_estimation": {"MWI": {"flash-floods": "&lt;p&gt;This indicator estimates potential economic damage based on global depth-damage functions provided by the JRC (refer to the publication at &lt;a target='_blank' hfref='https://op.europa.eu/en/publication-detail/-/publication/a20ecfa5-200e-11e7-84e2-01aa75ed71a1/language-en'&gt;https://op.europa.eu/en/publication-detail/-/publication/a20ecfa5-200e-11e7-84e2-01aa75ed71a1/language-en&lt;/a&gt;). The assessment differentiates damage according to water depth and land use, specifically utilizing the land use classes of urban and agricultural from the ESA WorldCover 2020 dataset (refer to the website &lt;a target='_blank' href='https://worldcover2020.esa.int/'&gt;https://worldcover2020.esa.int/&lt;/a&gt;). The monetary value is converted from Euro to Malawi Kwacha using a fixed exchange rate of xx.&lt;/p&gt;"}},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A35" s="8" t="s">
         <v>99</v>
       </c>
@@ -4239,7 +4237,7 @@
         <v>"dams": {"ZWE": {"drought": "This layer represents a selection of dams, and their associated reservoirs in Zimbabwe. The selection is made, based on the  Zimbabwe National Water Authority (ZINWA).&lt;br /&gt;&lt;br /&gt;Source Link Zimbabwe:&lt;ul&gt;&lt;li&gt;&lt;a target='_blank' href='https://www.zinwa.co.zw/dam-levels/'&gt;https://www.zinwa.co.zw/dam-levels/&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="8" t="s">
         <v>99</v>
       </c>
@@ -4305,7 +4303,7 @@
         <v>"dengue_cases_average": {"PHL": {"dengue": "Number of dengue cases per administrative division per year. &lt;br /&gt;&lt;br /&gt;Source: &lt;a target='_blank' href='https://doh.gov.ph/statistics'&gt;https://doh.gov.ph/statistics/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="73.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:19" ht="73.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="8" t="s">
         <v>99</v>
       </c>
@@ -4371,7 +4369,7 @@
         <v>"dengue_incidence_average": {"PHL": {"dengue": "Number of dengue cases per 10.000.000 people per administrative division per year. &lt;br /&gt;&lt;br /&gt;Source: &lt;a target='_blank' href='https://doh.gov.ph/statistics'&gt;https://doh.gov.ph/statistics/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="388.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:19" ht="393.45" x14ac:dyDescent="0.4">
       <c r="A38" s="8" t="s">
         <v>99</v>
       </c>
@@ -4461,7 +4459,7 @@
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:19" ht="189.45" x14ac:dyDescent="0.4">
       <c r="A39" s="8" t="s">
         <v>99</v>
       </c>
@@ -4549,7 +4547,7 @@
 &lt;br&gt;For further information please refer to the EAP"},</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:19" ht="262.3" x14ac:dyDescent="0.4">
       <c r="A40" s="8" t="s">
         <v>99</v>
       </c>
@@ -4619,7 +4617,7 @@
         <v>"ZWE": {"drought": "The drought vulnerability index is a composite index for the context of exposure to drought and the capacity to anticipate, cope with and recover from the impacts of droughts. The ZRCS selected nine main criteria:&lt;ul&gt;&lt;li&gt;14% Labor constrained households: 7 %unemployment rate 15+  and 7% economically non-active&lt;/li&gt;&lt;li&gt;15% Child, women and elderly headed households: 5% Female headed HH , 5% Head of Household (19-), 5% Head of Household (65+)&lt;/li&gt;&lt;li&gt;14% People with disabilities&lt;/li&gt;&lt;li&gt;15 % Pregnant and breast-feeding women, and children under five years: 5% pregnant women, 5% breast-feeding women, 5% children under five years&lt;/li&gt;&lt;li&gt;14 % Severe acute malnutrition&lt;/li&gt;&lt;li&gt;7% employment agriculture&lt;/li&gt;&lt;li&gt;7% cattle per km2&lt;/li&gt;&lt;li&gt;7% HIV prevalence&lt;/li&gt;&lt;li&gt;7% HIV ART Coverage&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A41" s="8" t="s">
         <v>99</v>
       </c>
@@ -4685,7 +4683,7 @@
         <v>"evacuation_centers": {"SSD": {"floods": "This layer shows the evacuation centres that can be used by the communities in case of a flood. They are shown as drop pins with an icon of a house with arrows pointing at it.&lt;br&gt;&lt;br&gt;&lt;strong&gt;Evacuation centres source&lt;/strong&gt;: South Sudan Red Cross Society (2022)."}},</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A42" s="8" t="s">
         <v>99</v>
       </c>
@@ -4753,7 +4751,7 @@
         <v>"exposed_pop_65": {"MWI": {"floods": "Number of Exposed Population 65+ is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is older than 65 years old.&lt;br&gt;&lt;br&gt;Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022."}},</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:19" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A43" s="8" t="s">
         <v>99</v>
       </c>
@@ -4819,7 +4817,7 @@
         <v>"exposed_pop_u18": {"MWI": {"floods": "Number of Exposed Population U18 is calculated by total target population living in the flood extent area within the administrative areas currently triggered. The target population are those living in the households classified as Poor, Poorer, Poorest and whose household head is below 18 years old.&lt;br&gt;&lt;br&gt;Source target population: Unified Beneficiary Registration (UBR). Department of Economy Planning and Development, Malawi. Collected and processed in 2022."}},</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A44" s="8" t="s">
         <v>99</v>
       </c>
@@ -4885,7 +4883,7 @@
         <v>"female_head_hh": {"UGA": {"floods": "Percentage of people living in female headed households.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a target='_blank' href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."}},</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A45" s="8" t="s">
         <v>99</v>
       </c>
@@ -4949,7 +4947,7 @@
         <v>"flood_extent": {"ETH": {"floods": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A46" s="8" t="s">
         <v>99</v>
       </c>
@@ -5019,7 +5017,7 @@
         <v>"KEN": {"floods": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="143.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:19" ht="143.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="8" t="s">
         <v>99</v>
       </c>
@@ -5033,13 +5031,13 @@
         <v>292</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="F47" s="22">
-        <v>45191</v>
+        <v>45281</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>331</v>
+        <v>345</v>
       </c>
       <c r="H47" s="18"/>
       <c r="I47" s="13" t="str">
@@ -5060,8 +5058,7 @@
       </c>
       <c r="M47" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>"flash-floods": "&lt;p&gt;This layer shows the area that is potentially flooding in this event. The fooded area is derived from the HEC-RAS flood model. The model resulted in scenario's that are related to the forecasted rainfall. The rainfall forecast from GFS is every 6 hours matched for each Traditional Authority to the scenario from the flood model.&lt;/p&gt;
-&lt;p&gt;The color indicates the depth of the flooded area, yellow means the area is only flooded with a shallow layer of water and red means a deep layer of water, with the different shades of orange somewhere in between.&lt;/p&gt;"</v>
+        <v>"flash-floods": "&lt;p&gt;This layer shows the potentially flooded area in the current event, determined by the HEC-RAS flood model. The model produces scenarios correlated with forecasted rainfall. GFS rainfall forecasts, updated every 6 hours, are synchronized with the flood model scenarios for each Traditional Authority.&lt;/p&gt;&lt;p&gt;The color scheme represents the depth of the flooded area: yellow signifies a shallow layer of water, red signifies a deep layer, and various shades of orange signifies intermediate depths.&lt;/p&gt;"</v>
       </c>
       <c r="N47" s="25" t="str">
         <f t="shared" si="5"/>
@@ -5085,11 +5082,10 @@
       </c>
       <c r="S47" s="12" t="str">
         <f t="shared" si="10"/>
-        <v>"MWI": {"flash-floods": "&lt;p&gt;This layer shows the area that is potentially flooding in this event. The fooded area is derived from the HEC-RAS flood model. The model resulted in scenario's that are related to the forecasted rainfall. The rainfall forecast from GFS is every 6 hours matched for each Traditional Authority to the scenario from the flood model.&lt;/p&gt;
-&lt;p&gt;The color indicates the depth of the flooded area, yellow means the area is only flooded with a shallow layer of water and red means a deep layer of water, with the different shades of orange somewhere in between.&lt;/p&gt;",</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+        <v>"MWI": {"flash-floods": "&lt;p&gt;This layer shows the potentially flooded area in the current event, determined by the HEC-RAS flood model. The model produces scenarios correlated with forecasted rainfall. GFS rainfall forecasts, updated every 6 hours, are synchronized with the flood model scenarios for each Traditional Authority.&lt;/p&gt;&lt;p&gt;The color scheme represents the depth of the flooded area: yellow signifies a shallow layer of water, red signifies a deep layer, and various shades of orange signifies intermediate depths.&lt;/p&gt;",</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A48" s="8" t="s">
         <v>99</v>
       </c>
@@ -5107,7 +5103,7 @@
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="6" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="H48" s="7">
         <v>44785</v>
@@ -5157,7 +5153,7 @@
         <v>"floods": "&lt;p&gt;The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 10-years) based on a global hydrological model.&lt;br&gt;&lt;br&gt;Source link: Flood hazard map of the World - 10-year return period. European Commission, Joint Research Centre (JRC). 2016. &lt;a target='_blank' href='https://data.jrc.ec.europa.eu/dataset/jrc-floods-floodmapgl_rp10y-tif'&gt;Flood hazard map of the World - 10-year return period - European Commission (europa.eu)&lt;/a&gt;.&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:19" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A49" s="8" t="s">
         <v>99</v>
       </c>
@@ -5233,7 +5229,7 @@
 covering it. "},</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:19" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A50" s="8" t="s">
         <v>99</v>
       </c>
@@ -5299,7 +5295,7 @@
         <v>"SSD": {"floods": "This layer shows the inundated area of recurring floods within a 5-year return period based on a global hydrological model. The flood extent is shown in red in the map.&lt;br&gt;&lt;br&gt;&lt;strong&gt;Flood extent source&lt;/strong&gt;: : The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A51" s="8" t="s">
         <v>99</v>
       </c>
@@ -5365,7 +5361,7 @@
         <v>"UGA": {"floods": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A52" s="8" t="s">
         <v>99</v>
       </c>
@@ -5429,7 +5425,7 @@
         <v>"ZMB": {"floods": "The flood extent layer indicates the inundated area of recurring floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."}},</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:19" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A53" s="8" t="s">
         <v>99</v>
       </c>
@@ -5495,7 +5491,7 @@
         <v>"flood_susceptibility": {"EGY": {"heavy-rain": "Flood susceptibility identifies the most vulnerable areas based on physical characteristics that determine the propensity for flooding” (Vojtek and Vojtekova, 2019). The mapping of flood susceptible areas involves the analysis of multiple criteria for different characteristics of the region that collectively contribute to the likelihood of floods.&lt;br/&gt;&lt;br/&gt;Nine influencing parameters based on a variety of satellite imagery and spatial datasets are the input factors of the model, such as topographical (Elevation model, Slope), physical (Land cover, Hydrological soil group) and hydrological properties (Height Above Nearest Drainage, Distance from Nearest Drainage, Topographic Wetness Index Slope, Rain intensity, Rain duration). Set of weights based on expert knowledge (The Analytical Hierarchical Process) from REACH (2019) was adapted in this analysis.&lt;br/&gt;&lt;br/&gt;&lt;strong&gt;LEGEND:&lt;/strong&gt; There are 4 classes of flood susceptibility. The higher the flood susceptibility, the darker blue the color.&lt;br/&gt;&lt;br/&gt;SOURCES:&lt;ul&gt;&lt;li&gt;REACH. Yemen Flood Susceptibility. 2019. &lt;a target='_blank' href='https://reliefweb.int/sites/reliefweb.int/files/resources/REACH_YEM_MethodologyNote_HVA_FloodSusceptibility_01APR2020_EN_V2.pdf'&gt;https://reliefweb.int/sites/reliefweb.int/files/resources/REACH_YEM_MethodologyNote_HVA_FloodSusceptibility_01APR2020_EN_V2.pdf&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Vojtek, M.; Vojteková, J. Flood Susceptibility Mapping on a National Scale in Slovakia Using the Analytical Hierarchy Process. Water 2019, 11, 364. &lt;a target='_blank' href='https://doi.org/10.3390/w11020364'&gt;https://doi.org/10.3390/w11020364&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:19" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A54" s="8" t="s">
         <v>99</v>
       </c>
@@ -5565,7 +5561,7 @@
         <v>"flood_vulnerability_index": {"KEN": {"floods": "&lt;p&gt;The flood vulnerability index is a composite index for the context of exposure to floods and the capacity to anticipate, cope with and recover from the impacts of floods. The National Society and Technical Working group selected the following criteria below:&lt;/p&gt;&lt;ul&gt;    &lt;li&gt;18.8% age under 5&amp;nbsp;&lt;/li&gt; &lt;li&gt;15.4% age over 65&lt;/li&gt; &lt;li&gt;18.2% poverty index&lt;/li&gt;&lt;li&gt;19.3% Gini Index&lt;/li&gt;&lt;li&gt;12.3% strong wall type&lt;/li&gt;&lt;li&gt;36.3%travel time to the nearest city&lt;/li&gt; &lt;li&gt;16.0% access to improved water sources&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;For further information please refer to the EAP&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A55" s="8" t="s">
         <v>99</v>
       </c>
@@ -5631,7 +5627,7 @@
         <v>"MWI": {"floods": "The flood vulnerability index is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts of floods. The vulnerability index is selected with the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Flood physical exposure. &lt;/li&gt;&lt;li&gt; 20% Poverty: Poverty incidence &lt;/li&gt;&lt;li&gt;20% Gender: Female headed household &lt;/li&gt;&lt;li&gt;20% Age: Population below 5 years &lt;/li&gt;&lt;li&gt;20 % Disability: People with disability&lt;/li&gt;&lt;/ul&gt;."},</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A56" s="8" t="s">
         <v>99</v>
       </c>
@@ -5697,12 +5693,12 @@
         <v>"UGA": {"floods": "The disaster vulnerability index is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts of floods. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For further information please refer to the EAP. For source links, see each individual layer."}},</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A57" s="8" t="s">
         <v>99</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>183</v>
@@ -5713,7 +5709,7 @@
       <c r="E57" s="20"/>
       <c r="F57" s="5"/>
       <c r="G57" s="6" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
       <c r="H57" s="18"/>
       <c r="I57" s="13" t="str">
@@ -5761,7 +5757,7 @@
         <v>"gauges": {"MWI": {"flash-floods": "The river gauge layer shows you the location of river gauges on the map, they are visualised as blue drop pins with a river icon. Clicking on a drop pin opens a pop up containing information about the current water level in meters above sea level (mMSL) this is measured daily with the latest model run. The difference compared to 24 hours ago is shown in green for decrease or red for increase. The reference water level is the typical level for this station during this season."}},</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:19" ht="204" x14ac:dyDescent="0.4">
       <c r="A58" s="8" t="s">
         <v>99</v>
       </c>
@@ -5825,7 +5821,7 @@
         <v>"glofas_stations": {"ETH": {"floods": "This layer shows the locations of the Global Flood Awareness System (GloFAS) stations. These stations are shown as drop pins with a trigger hazard icon on the map. The drop pins can be shown in &lt;strong&gt;navy&lt;/strong&gt; for below threshold or &lt;strong&gt;purple&lt;/strong&gt; for above threshold depending on the level of river discharge measured.&lt;br&gt;The GloFAS forecast is used for the trigger. These forecasts are often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 75% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a target='_blank' href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:19" ht="204" x14ac:dyDescent="0.4">
       <c r="A59" s="8" t="s">
         <v>99</v>
       </c>
@@ -5893,7 +5889,7 @@
         <v>"KEN": {"floods": "This layer shows the locations of the Global Flood Awareness System (GloFAS) stations. These stations are shown as drop pins with a trigger hazard icon on the map. The drop pins can be shown in &lt;strong&gt;navy&lt;/strong&gt; for below threshold or &lt;strong&gt;purple&lt;/strong&gt; for above threshold depending on the level of river discharge measured.&lt;br&gt;The GloFAS forecast is used for the trigger. These forecasts are often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 85% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a target='_blank' href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:19" ht="204" x14ac:dyDescent="0.4">
       <c r="A60" s="8" t="s">
         <v>99</v>
       </c>
@@ -5959,7 +5955,7 @@
         <v>"MWI": {"floods": "This layer shows the locations of the Global Flood Awareness System (GloFAS) stations. These stations are shown as drop pins with a trigger hazard icon on the map. The drop pins can be shown in &lt;strong&gt;navy&lt;/strong&gt; for below threshold or &lt;strong&gt;purple&lt;/strong&gt; for above threshold depending on the level of river discharge measured.&lt;br&gt;The GloFAS forecast is used for the trigger. These forecasts are often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 6 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a target='_blank' href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:19" ht="204" x14ac:dyDescent="0.4">
       <c r="A61" s="8" t="s">
         <v>99</v>
       </c>
@@ -6023,7 +6019,7 @@
         <v>"PHL": {"floods": "This layer shows the locations of the Global Flood Awareness System (GloFAS) stations. These stations are shown as drop pins with a trigger hazard icon on the map. The drop pins can be shown in &lt;strong&gt;navy&lt;/strong&gt; for below threshold or &lt;strong&gt;purple&lt;/strong&gt; for above threshold depending on the level of river discharge measured.&lt;br&gt;The GloFAS forecast is used for the trigger. These forecasts are often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 3 days ahead in this layer) for the large river basins. The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 70% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a target='_blank' href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:19" ht="204" x14ac:dyDescent="0.4">
       <c r="A62" s="8" t="s">
         <v>99</v>
       </c>
@@ -6087,7 +6083,7 @@
         <v>"SSD": {"floods": "This layer shows the locations of the Global Flood Awareness System (GloFAS) stations. These stations are shown as drop pins with a trigger hazard icon on the map. The drop pins can be shown in &lt;strong&gt;navy&lt;/strong&gt; for below threshold or &lt;strong&gt;purple&lt;/strong&gt; for above threshold depending on the level of river discharge measured.&lt;br&gt;The GloFAS forecast is used for the trigger. These forecasts are often used by the National Governmental Meteorological Services.&lt;br&gt;&lt;br&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast and monitoring system that delivers global ensemble river discharge forecasts (limited up to 3 days ahead in this layer) for the large river basins. The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br&gt;&lt;br&gt;The methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60% trigger-threshold discharge levels is presented as the 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to specific GloFAS Stations, and as such they determine which areas are triggered when the stations reach /exceed the trigger threshold value (for more information see the EAP in ‘about trigger’).&lt;br&gt;&lt;br&gt;&lt;strong&gt;Glofas stations source&lt;/strong&gt;: &lt;a target='_blank' href=‘https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:19" ht="204" x14ac:dyDescent="0.4">
       <c r="A63" s="8" t="s">
         <v>99</v>
       </c>
@@ -6153,7 +6149,7 @@
         <v>"UGA": {"floods": "This layer shows the locations of the Global Flood Awareness System (GloFAS) stations. These stations are shown as drop pins with a trigger hazard icon on the map. The drop pins can be shown in &lt;strong&gt;navy&lt;/strong&gt; for below threshold or &lt;strong&gt;purple&lt;/strong&gt; for above threshold depending on the level of river discharge measured.&lt;br&gt;The GloFAS forecast is used for the trigger. These forecasts are often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a target='_blank' href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:19" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A64" s="8" t="s">
         <v>99</v>
       </c>
@@ -6217,7 +6213,7 @@
         <v>"ZMB": {"floods": "This layer shows the locations of the Global Flood Awareness System (GloFAS) stations. These stations are shown as drop pins with a trigger hazard icon on the map. The drop pins can be shown in &lt;strong&gt;navy&lt;/strong&gt; for below threshold, &lt;strong&gt;yellow&lt;/strong&gt; (minimal risk), &lt;strong&gt;orange&lt;/strong&gt; (medium risk) and &lt;strong&gt;purple&lt;/strong&gt; (above threshold - trigger) depending on the level of river discharge measured.&lt;br&gt;The GloFAS forecast is used for the trigger. These forecasts are often used by the National Governmental Meteorological Services.&lt;br /&gt;&lt;br /&gt;GloFAS version 3.1 is a global integrated hydro-meteorological forecast- and monitoring system that delivers global ensemble river discharge forecasts (limited up to 5 days ahead in this layer) for the large river basins (greater than 1000 km2). The GloFAS 3.1 is based on the LISFLOOD hydrological model.&lt;br /&gt;&lt;br /&gt;Methodology presenting the GloFAS probability levels: Methodology presenting the GloFAS probability levels: The ECMWF-ENS meteorological forecast data contains a 51-member ensemble. The 60/70/80% trigger-threshold discharge levels are presented as 'trigger-alert' levels agreed on in the EAP. The probability is the percentage of the 51 ensemble members that predicts that the discharge is above the threshold. The administrative areas in the corresponding country are mapped to a specific GloFAS Station, and as such it is determined which areas are triggered when the station exceeds the trigger threshold value (for more informatie see the EAP).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a target='_blank' href='https://www.globalfloods.eu/'&gt;https://www.globalfloods.eu/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A65" s="8" t="s">
         <v>99</v>
       </c>
@@ -6281,7 +6277,7 @@
         <v>"grassland": {"ETH": {"drought": "This layer represents the grassland. It is visualised in green on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Grassland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010",</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A66" s="8" t="s">
         <v>99</v>
       </c>
@@ -6345,7 +6341,7 @@
         <v>"floods": "This layer represents the grassland. It is visualised in green on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Grassland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:19" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A67" s="8" t="s">
         <v>99</v>
       </c>
@@ -6413,7 +6409,7 @@
         <v>"KEN": {"floods": "This layer represents the grassland. It is visualised in green on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Grassland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A68" s="8" t="s">
         <v>99</v>
       </c>
@@ -6477,7 +6473,7 @@
         <v>"UGA": {"drought": "This layer represents the grassland. It is visualised in green on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Grassland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010",</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A69" s="8" t="s">
         <v>99</v>
       </c>
@@ -6543,7 +6539,7 @@
         <v>"floods": "This layer represents the grassland. It is visualised in green on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Grassland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A70" s="8" t="s">
         <v>99</v>
       </c>
@@ -6607,7 +6603,7 @@
         <v>"ZMB": {"drought": "This layer represents the grassland. It is visualised in green on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Grassland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010",</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A71" s="8" t="s">
         <v>99</v>
       </c>
@@ -6671,7 +6667,7 @@
         <v>"floods": "This layer represents the grassland. It is visualised in green on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Grassland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"},</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A72" s="8" t="s">
         <v>99</v>
       </c>
@@ -6737,7 +6733,7 @@
         <v>"ZWE": {"drought": "This layer represents the grassland. It is visualised in green on the map. The land use classes are based on GLOBCOVER Land Cover Classifications.&lt;br /&gt;&lt;br /&gt;Combined grassland; consists of two land-use types.&lt;ol&gt;&lt;li&gt;Mosaic forest or shrubland - 50-70% (forest/shrubland &amp; 20-50% grassland&lt;/li&gt;&lt;li&gt;Mosaic grassland - 50-70% grassland &amp; 20-50% forest or shrubland&lt;/li&gt;&lt;/ol&gt;&lt;br /&gt;Grassland source: © ESA 2010 and UCLouvain. Accompanied by a link to our ESA DUE GlobCover website: &lt;a target='_blank' href='http://due.esrin.esa.int/page_globcover.php'&gt;http://due.esrin.esa.int/page_globcover.php&lt;/a&gt;. Year: 2010"}},</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A73" s="8" t="s">
         <v>99</v>
       </c>
@@ -6803,7 +6799,7 @@
         <v>"health_sites": {"ETH": {"drought": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a target='_blank' href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;",</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A74" s="8" t="s">
         <v>99</v>
       </c>
@@ -6867,7 +6863,7 @@
         <v>"floods": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a target='_blank' href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;",</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A75" s="8" t="s">
         <v>99</v>
       </c>
@@ -6931,7 +6927,7 @@
         <v>"malaria": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a target='_blank' href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;"},</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="105" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:19" ht="105" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" s="8" t="s">
         <v>99</v>
       </c>
@@ -7003,7 +6999,7 @@
 &lt;p&gt;&lt;strong&gt;Source link&lt;/strong&gt;: &lt;a target='_blank' href='https://healthsites.io/'&gt;https://healthsites.io/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A77" s="8" t="s">
         <v>99</v>
       </c>
@@ -7017,13 +7013,13 @@
         <v>292</v>
       </c>
       <c r="E77" s="20" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="F77" s="22">
-        <v>45191</v>
+        <v>45281</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="H77" s="18"/>
       <c r="I77" s="13" t="str">
@@ -7044,7 +7040,7 @@
       </c>
       <c r="M77" s="12" t="str">
         <f t="shared" si="15"/>
-        <v>"flash-floods": "&lt;p&gt;This layer shows the Health Sites in the potentially affected Traditional Authorities. Each Health Site has either a blue or a red marker. Blue when it is outside the potentially inundated area so safe and red when it is inside the potentially inundated area so in danger.&lt;/p&gt;
+        <v>"flash-floods": "&lt;p&gt;This layer shows Health Sites within Traditional Authorities that may be affected. Each Health Site is marked with either a blue or red indicator. Blue indicates it is outside the potentially inundated area and safe. Red indicates it is inside the potentially inundated area and at risk.&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: Cloud2Street&lt;/p&gt;"</v>
       </c>
@@ -7070,12 +7066,12 @@
       </c>
       <c r="S77" s="12" t="str">
         <f t="shared" si="21"/>
-        <v>"MWI": {"flash-floods": "&lt;p&gt;This layer shows the Health Sites in the potentially affected Traditional Authorities. Each Health Site has either a blue or a red marker. Blue when it is outside the potentially inundated area so safe and red when it is inside the potentially inundated area so in danger.&lt;/p&gt;
+        <v>"MWI": {"flash-floods": "&lt;p&gt;This layer shows Health Sites within Traditional Authorities that may be affected. Each Health Site is marked with either a blue or red indicator. Blue indicates it is outside the potentially inundated area and safe. Red indicates it is inside the potentially inundated area and at risk.&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: Cloud2Street&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A78" s="8" t="s">
         <v>99</v>
       </c>
@@ -7141,7 +7137,7 @@
         <v>"PHL": {"dengue": "Health facilities by type and location. Health facility types &lt;strong&gt;hospital&lt;/strong&gt; and &lt;strong&gt;clinic&lt;/strong&gt; are shown with different markers. Other types are omitted and rare in the data.&lt;br /&gt;&lt;br /&gt;Source: &lt;a target='_blank' href='https://healthsites.io/'&gt;https://healthsites.io/&lt;a/&gt;",</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A79" s="8" t="s">
         <v>99</v>
       </c>
@@ -7155,7 +7151,7 @@
         <v>139</v>
       </c>
       <c r="E79" s="20" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F79" s="5"/>
       <c r="G79" s="6" t="s">
@@ -7217,7 +7213,7 @@
 &lt;a target='_blank' href='https://healthsites.io/'&gt;https://healthsites.io/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A80" s="8" t="s">
         <v>99</v>
       </c>
@@ -7291,7 +7287,7 @@
 &lt;a target='_blank' href='https://healthsites.io/'&gt;https://healthsites.io/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A81" s="8" t="s">
         <v>99</v>
       </c>
@@ -7359,7 +7355,7 @@
         <v>"Hotspot_General": {"ETH": {"drought": "Area of Concern or Hotspot is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on food, livelihood and nutrition insecurity and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response (related to water, human health, education, seed, livestock health and feed)",</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A82" s="8" t="s">
         <v>99</v>
       </c>
@@ -7425,7 +7421,7 @@
         <v>"floods": "Area of Concern or Hotspot is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on food, livelihood and nutrition insecurity and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response (related to water, human health, education, seed, livestock health and feed)",</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A83" s="8" t="s">
         <v>99</v>
       </c>
@@ -7493,7 +7489,7 @@
         <v>"malaria": "Area of Concern or Hotspot is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on food, livelihood and nutrition insecurity and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response (related to water, human health, education, seed, livestock health and feed)"}},</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A84" s="8" t="s">
         <v>99</v>
       </c>
@@ -7561,7 +7557,7 @@
         <v>"Hotspot_Health": {"ETH": {"malaria": "Area of Concern or Hotspot for health is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on health and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response"}},</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A85" s="8" t="s">
         <v>99</v>
       </c>
@@ -7627,7 +7623,7 @@
         <v>"Hotspot_Nutrition": {"ETH": {"drought": "Area of Concern or Hotspot for nutrition is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on nutrition insecurity and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response"}},</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A86" s="8" t="s">
         <v>99</v>
       </c>
@@ -7695,7 +7691,7 @@
         <v>"Hotspot_Water": {"ETH": {"drought": "Area of Concern or Hotspot for Water is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on WASH and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response",</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A87" s="8" t="s">
         <v>99</v>
       </c>
@@ -7761,7 +7757,7 @@
         <v>"floods": "Area of Concern or Hotspot for Water is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on WASH and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response",</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A88" s="8" t="s">
         <v>99</v>
       </c>
@@ -7829,7 +7825,7 @@
         <v>"malaria": "Area of Concern or Hotspot for Water is defined as: an area or population affected by any undesirable events or situations that have an immediate or in the near future direct bearing on WASH and require immediate attention or intervention that could be assessments, close monitoring or appropriate food or non-food response"}},</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A89" s="8" t="s">
         <v>99</v>
       </c>
@@ -7895,7 +7891,7 @@
         <v>"houses_affected": {"PHL": {"typhoon": "&lt;p&gt;Total Number of completely  damaged houses as predicted by 510 typhoon impact prediction model&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A90" s="8" t="s">
         <v>99</v>
       </c>
@@ -7959,7 +7955,7 @@
         <v>"IPC_forecast_long": {"ETH": {"drought": "This layer represents the IPC (Integrated food security Phase Classification). It is visualised in shades of grey or purple on the map depending on if there is a trigger. IPC long forecast: Most likely food security outcomes -  the medium-term projection &lt;a target='_blank' href='https://fews.net/about/integrated-phase-classification'&gt;https://fews.net/about/integrated-phase-classification&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A91" s="8" t="s">
         <v>99</v>
       </c>
@@ -8025,7 +8021,7 @@
         <v>"malaria": "This layer represents the IPC (Integrated food security Phase Classification). It is visualised in shades of grey or purple on the map depending on if there is a trigger. IPC long forecast: Most likely food security outcomes -  the medium-term projection &lt;a target='_blank' href='https://fews.net/about/integrated-phase-classification'&gt;https://fews.net/about/integrated-phase-classification&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A92" s="8" t="s">
         <v>99</v>
       </c>
@@ -8089,7 +8085,7 @@
         <v>"UGA": {"drought": "This layer represents the IPC (Integrated food security Phase Classification). It is visualised in shades of grey or purple on the map depending on if there is a trigger. IPC long forecast: Most likely food security outcomes -  the medium-term projection &lt;a target='_blank' href='https://fews.net/about/integrated-phase-classification'&gt;https://fews.net/about/integrated-phase-classification&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A93" s="8" t="s">
         <v>99</v>
       </c>
@@ -8155,7 +8151,7 @@
         <v>"IPC_forecast_short": {"ETH": {"floods": "This layer represents the IPC (Integrated food security Phase Classification). It is visualised in shades of grey or purple on the map depending on if there is a trigger. IPC short forecast: Most likely food security outcomes -  the near-term projection &lt;a target='_blank' href='https://fews.net/about/integrated-phase-classification'&gt;https://fews.net/about/integrated-phase-classification&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:19" ht="204" x14ac:dyDescent="0.4">
       <c r="A94" s="8" t="s">
         <v>99</v>
       </c>
@@ -8231,7 +8227,7 @@
 &lt;p&gt;Latest updated: every month&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A95" s="8" t="s">
         <v>99</v>
       </c>
@@ -8297,7 +8293,7 @@
         <v>"malaria_risk": {"ETH": {"malaria": "Malaria risk:Spatial limits of Plasmodium vivax malaria transmission (0-none 2- high)  &lt;a target='_blank' href='https://malariaatlas.org/'&gt;https://malariaatlas.org/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A96" s="8" t="s">
         <v>99</v>
       </c>
@@ -8363,7 +8359,7 @@
         <v>"malaria_suitable_temperature": {"ETH": {"malaria": "Malaria suitability:Temperature suitability index for Plasmodium vivax transmission, 2010 &lt;a target='_blank' href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A97" s="8" t="s">
         <v>99</v>
       </c>
@@ -8429,7 +8425,7 @@
         <v>"motorized_travel_time_to_health": {"ETH": {"malaria": "Access to Health with vehicle: Estimated travel time (minutes) to the nearest healthcare facility, with motorized vehicle &lt;a target='_blank' href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A98" s="8" t="s">
         <v>99</v>
       </c>
@@ -8443,13 +8439,13 @@
         <v>292</v>
       </c>
       <c r="E98" s="20" t="s">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="F98" s="22">
-        <v>45191</v>
+        <v>45281</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H98" s="18"/>
       <c r="I98" s="13" t="str">
@@ -8470,7 +8466,7 @@
       </c>
       <c r="M98" s="12" t="str">
         <f t="shared" si="15"/>
-        <v>"flash-floods": "&lt;p&gt;This indicator shows the total number of buildings in the potentially flooded area. The number is filtered on the selected area (see above).&lt;/p&gt;
+        <v>"flash-floods": "&lt;p&gt;This indicator shows the total number of buildings within the potentially flooded area, filtered based on the selected area (see above).&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: Openstreetmap&lt;/p&gt;"</v>
       </c>
@@ -8496,12 +8492,12 @@
       </c>
       <c r="S98" s="12" t="str">
         <f t="shared" si="21"/>
-        <v>"nr_affected_buildings": {"MWI": {"flash-floods": "&lt;p&gt;This indicator shows the total number of buildings in the potentially flooded area. The number is filtered on the selected area (see above).&lt;/p&gt;
+        <v>"nr_affected_buildings": {"MWI": {"flash-floods": "&lt;p&gt;This indicator shows the total number of buildings within the potentially flooded area, filtered based on the selected area (see above).&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: Openstreetmap&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A99" s="8" t="s">
         <v>99</v>
       </c>
@@ -8515,13 +8511,13 @@
         <v>292</v>
       </c>
       <c r="E99" s="20" t="s">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="F99" s="22">
-        <v>45191</v>
+        <v>45281</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="H99" s="18"/>
       <c r="I99" s="13" t="str">
@@ -8542,7 +8538,7 @@
       </c>
       <c r="M99" s="12" t="str">
         <f t="shared" si="15"/>
-        <v>"flash-floods": "&lt;p&gt;This indicator shows the total number of health sites in the potentially flooded area. The number is filtered on the selected area (see above).&lt;/p&gt;
+        <v>"flash-floods": "&lt;p&gt;This indicator shows the total number of health sites in the potentially flooded area, Filtered based on the selected area (see above).&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: Cloud2Street&lt;/p&gt;"</v>
       </c>
@@ -8568,12 +8564,12 @@
       </c>
       <c r="S99" s="12" t="str">
         <f t="shared" si="21"/>
-        <v>"nr_affected_clinics": {"MWI": {"flash-floods": "&lt;p&gt;This indicator shows the total number of health sites in the potentially flooded area. The number is filtered on the selected area (see above).&lt;/p&gt;
+        <v>"nr_affected_clinics": {"MWI": {"flash-floods": "&lt;p&gt;This indicator shows the total number of health sites in the potentially flooded area, Filtered based on the selected area (see above).&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: Cloud2Street&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A100" s="8" t="s">
         <v>99</v>
       </c>
@@ -8587,13 +8583,13 @@
         <v>292</v>
       </c>
       <c r="E100" s="20" t="s">
-        <v>335</v>
+        <v>352</v>
       </c>
       <c r="F100" s="22">
-        <v>45191</v>
+        <v>45281</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="H100" s="18"/>
       <c r="I100" s="13" t="str">
@@ -8614,7 +8610,7 @@
       </c>
       <c r="M100" s="12" t="str">
         <f t="shared" si="15"/>
-        <v>"flash-floods": "&lt;p&gt;This indicator shows the total amount of kilometers of roads in the potentially flooded area. The number is filtered on the selected area (see above). The roads are not filtered on the type of road so it includes more roads than the map layer.&lt;/p&gt;
+        <v>"flash-floods": "&lt;p&gt;This indicator shows the total amount of kilometers of roads in the potentially flooded area, Filtered based on the selected area (see above). The roads are not filtered by the type of road so it includes more roads than is shown in the map layer.&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: Openstreetmap&lt;/p&gt;"</v>
       </c>
@@ -8640,12 +8636,12 @@
       </c>
       <c r="S100" s="12" t="str">
         <f t="shared" si="21"/>
-        <v>"nr_affected_roads": {"MWI": {"flash-floods": "&lt;p&gt;This indicator shows the total amount of kilometers of roads in the potentially flooded area. The number is filtered on the selected area (see above). The roads are not filtered on the type of road so it includes more roads than the map layer.&lt;/p&gt;
+        <v>"nr_affected_roads": {"MWI": {"flash-floods": "&lt;p&gt;This indicator shows the total amount of kilometers of roads in the potentially flooded area, Filtered based on the selected area (see above). The roads are not filtered by the type of road so it includes more roads than is shown in the map layer.&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: Openstreetmap&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A101" s="8" t="s">
         <v>99</v>
       </c>
@@ -8659,13 +8655,13 @@
         <v>292</v>
       </c>
       <c r="E101" s="20" t="s">
-        <v>338</v>
+        <v>354</v>
       </c>
       <c r="F101" s="22">
-        <v>45191</v>
+        <v>45281</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="H101" s="18"/>
       <c r="I101" s="13" t="str">
@@ -8686,7 +8682,7 @@
       </c>
       <c r="M101" s="12" t="str">
         <f t="shared" si="15"/>
-        <v>"flash-floods": "&lt;p&gt;This indicator shows the total number of school buildings in the potentially flooded area. The number is filtered on the selected area (see above).&lt;/p&gt;
+        <v>"flash-floods": "&lt;p&gt;This indicator shows the total number of school buildings in the potentially flooded area, Filtered based on the selected area (see above).&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: Cloud2Street&lt;/p&gt;"</v>
       </c>
@@ -8712,12 +8708,12 @@
       </c>
       <c r="S101" s="12" t="str">
         <f t="shared" si="21"/>
-        <v>"nr_affected_schools": {"MWI": {"flash-floods": "&lt;p&gt;This indicator shows the total number of school buildings in the potentially flooded area. The number is filtered on the selected area (see above).&lt;/p&gt;
+        <v>"nr_affected_schools": {"MWI": {"flash-floods": "&lt;p&gt;This indicator shows the total number of school buildings in the potentially flooded area, Filtered based on the selected area (see above).&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: Cloud2Street&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A102" s="8" t="s">
         <v>99</v>
       </c>
@@ -8731,13 +8727,13 @@
         <v>292</v>
       </c>
       <c r="E102" s="20" t="s">
-        <v>339</v>
+        <v>356</v>
       </c>
       <c r="F102" s="22">
-        <v>45191</v>
+        <v>45281</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="H102" s="18"/>
       <c r="I102" s="13" t="str">
@@ -8758,7 +8754,7 @@
       </c>
       <c r="M102" s="12" t="str">
         <f t="shared" si="15"/>
-        <v>"flash-floods": "&lt;p&gt;This indicator shows the total number of water points in the potentially flooded area. The number is filtered on the selected area (see above).&lt;/p&gt;
+        <v>"flash-floods": "&lt;p&gt;This indicator shows the total number of water points in the potentially flooded area, Filtered based on the selected area (see above).&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: &lt;a target='_blank' href='https://portal.mwater.co/#/'&gt;mWater &lt;/a&gt;&lt;/p&gt;"</v>
       </c>
@@ -8784,12 +8780,12 @@
       </c>
       <c r="S102" s="12" t="str">
         <f t="shared" si="21"/>
-        <v>"nr_affected_waterpoints": {"MWI": {"flash-floods": "&lt;p&gt;This indicator shows the total number of water points in the potentially flooded area. The number is filtered on the selected area (see above).&lt;/p&gt;
+        <v>"nr_affected_waterpoints": {"MWI": {"flash-floods": "&lt;p&gt;This indicator shows the total number of water points in the potentially flooded area, Filtered based on the selected area (see above).&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: &lt;a target='_blank' href='https://portal.mwater.co/#/'&gt;mWater &lt;/a&gt;&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A103" s="8" t="s">
         <v>99</v>
       </c>
@@ -8853,7 +8849,7 @@
         <v>"population": {"EGY": {"heavy-rain": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A104" s="8" t="s">
         <v>99</v>
       </c>
@@ -8919,7 +8915,7 @@
         <v>"ETH": {"drought": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A105" s="8" t="s">
         <v>99</v>
       </c>
@@ -8983,7 +8979,7 @@
         <v>"floods": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A106" s="8" t="s">
         <v>99</v>
       </c>
@@ -9055,7 +9051,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A107" s="8" t="s">
         <v>99</v>
       </c>
@@ -9127,7 +9123,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A108" s="8" t="s">
         <v>99</v>
       </c>
@@ -9195,7 +9191,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; peanutButter: An R package to produce rapid-response gridded population estimates from building footprints, version 1.0.0 version 1.0.0. Accessed 15-08-2022. WorldPop, University of Southampton. 2021. &amp;nbsp;&lt;a target='_blank' href='https://apps.worldpop.org/peanutButter/'&gt;https://apps.worldpop.org/peanutButter/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="270" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:19" ht="270" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A109" s="8" t="s">
         <v>99</v>
       </c>
@@ -9263,7 +9259,7 @@
 &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A110" s="8" t="s">
         <v>99</v>
       </c>
@@ -9329,7 +9325,7 @@
         <v>"SSD": {"floods": "This layer shows the population’s location in the country, visualised in grey on the map.&lt;br&gt;&lt;br&gt;&lt;strong&gt;Population data source&lt;/strong&gt;: WorldPop (&lt;a target='_blank' href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt; - School of Geography and Environmental Science, University of Southampton; Department of Geography and Geosciences, University of Louisville; Departement de Geographie, Universite de Namur) and Center for International Earth Science Information Network (CIESIN), Columbia University (2018)."},</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A111" s="8" t="s">
         <v>99</v>
       </c>
@@ -9397,7 +9393,7 @@
 &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A112" s="8" t="s">
         <v>99</v>
       </c>
@@ -9463,7 +9459,7 @@
         <v>"floods": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A113" s="8" t="s">
         <v>99</v>
       </c>
@@ -9529,7 +9525,7 @@
 &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A114" s="8" t="s">
         <v>99</v>
       </c>
@@ -9593,7 +9589,7 @@
         <v>"ZMB": {"drought": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A115" s="8" t="s">
         <v>99</v>
       </c>
@@ -9657,7 +9653,7 @@
         <v>"floods": "The population data comes from the following source: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:19" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A116" s="8" t="s">
         <v>99</v>
       </c>
@@ -9727,7 +9723,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;The population data comes from the following source: Worldpop data:&amp;nbsp;&lt;a target='_blank' href='https://www.worldpop.org/geodata/'&gt;https://www.worldpop.org/geodata/&lt;/a&gt;&lt;/p&gt; &lt;p&gt;Accessed 07-2020 The mapping approach is Pezzulo, C., Hornby, G., Sorichetta, A. et al. Sub-national mapping of population pyramids and dependency ratios in Africa and Asia. Sci Data 4, 170089 (2017). &lt;a target='_blank' href='https://doi.org/10.1038/sdata.2017.89'&gt;https://doi.org/10.1038/sdata.2017.89&lt;/a&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:19" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A117" s="8" t="s">
         <v>99</v>
       </c>
@@ -9793,7 +9789,7 @@
         <v>"population_affected": {"EGY": {"heavy-rain": "Number of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."},</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A118" s="8" t="s">
         <v>99</v>
       </c>
@@ -9859,7 +9855,7 @@
         <v>"ETH": {"drought": "Number of people exposed is calculated by the population living within the districts currently triggered. The number of people data is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A119" s="8" t="s">
         <v>99</v>
       </c>
@@ -9923,7 +9919,7 @@
         <v>"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:19" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A120" s="8" t="s">
         <v>99</v>
       </c>
@@ -10003,7 +9999,7 @@
 &lt;/ul&gt;",</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:19" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A121" s="8" t="s">
         <v>99</v>
       </c>
@@ -10085,7 +10081,7 @@
 &lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A122" s="8" t="s">
         <v>99</v>
       </c>
@@ -10099,13 +10095,13 @@
         <v>292</v>
       </c>
       <c r="E122" s="20" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
       <c r="F122" s="22">
-        <v>45191</v>
+        <v>45281</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>346</v>
+        <v>359</v>
       </c>
       <c r="H122" s="18"/>
       <c r="I122" s="13" t="str">
@@ -10126,7 +10122,7 @@
       </c>
       <c r="M122" s="12" t="str">
         <f t="shared" si="15"/>
-        <v>"flash-floods": "&lt;p&gt;This layer shows the amount of people that is potentially exposed per geographic area. This is calculated by determining the amount of people that live in the potentially flooded area.&lt;/p&gt;
+        <v>"flash-floods": "&lt;p&gt;This layer shows the amount of people that is potentially exposed per geographic area. This is calculated by determining the amount of people who live in the potentially flooded area.&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: &lt;a target='_blank' href='https://data.humdata.org/dataset/highresolutionpopulationdensitymaps-mwi'&gt;Meta on HDX &lt;/a&gt;&lt;/p&gt;"</v>
       </c>
@@ -10152,12 +10148,12 @@
       </c>
       <c r="S122" s="12" t="str">
         <f t="shared" si="21"/>
-        <v>"MWI": {"flash-floods": "&lt;p&gt;This layer shows the amount of people that is potentially exposed per geographic area. This is calculated by determining the amount of people that live in the potentially flooded area.&lt;/p&gt;
+        <v>"MWI": {"flash-floods": "&lt;p&gt;This layer shows the amount of people that is potentially exposed per geographic area. This is calculated by determining the amount of people who live in the potentially flooded area.&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Source: &lt;a target='_blank' href='https://data.humdata.org/dataset/highresolutionpopulationdensitymaps-mwi'&gt;Meta on HDX &lt;/a&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A123" s="8" t="s">
         <v>99</v>
       </c>
@@ -10173,7 +10169,7 @@
       <c r="E123" s="20"/>
       <c r="F123" s="5"/>
       <c r="G123" s="6" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="H123" s="7">
         <v>44798</v>
@@ -10223,7 +10219,7 @@
         <v>"floods": "&lt;p&gt;Number of people exposed is calculated by the population living in the flood extent area within the administrative areas currently triggered. The number of people and the flood extent are derived from the below sources.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;    &lt;li&gt;Source (Population Data): peanutButter: An R package to produce rapid-response gridded population estimates from building footprints, version 1.0.0 version 1.0.0. Accessed 15-08-2022. WorldPop, University of Southampton. 2021. &amp;nbsp;&lt;a target='_blank' href='https://apps.worldpop.org/peanutButter/'&gt;https://apps.worldpop.org/peanutButter/&lt;/a&gt;&lt;/li&gt;    &lt;li&gt;Source Flood Extent: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:19" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A124" s="8" t="s">
         <v>99</v>
       </c>
@@ -10239,7 +10235,7 @@
       <c r="E124" s="20"/>
       <c r="F124" s="5"/>
       <c r="G124" s="6" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="H124" s="7">
         <v>44663</v>
@@ -10289,7 +10285,7 @@
         <v>"PHL": {"floods": "&lt;p&gt;Number of people exposed is calculated by the population living in the flood extent area within the manucipality currently triggered. The number of people and the flood extent are derived from the below sources.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Source (Population Data): High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Source Flood Extent: The flood extent maps are generated by the National Operational Assesment of Hazards(NOAH) project.&lt;a target='_blank' href='https://noah.up.edu.ph/'&gt;https://noah.up.edu.ph/&lt;/a&gt; The 25-year rain return flood hazard maps show low, medium, and high flood hazards represented as yellow, orange, and red respectively. Flood hazards consider take both the height and velocity of the water into consideration and calculates the hazard levels based on the danger they pose to people and structures. Generally, for an average Filipino with a height of 5’ 6”, areas with flood depths from the knee down can be considered to have low hazard levels. Those with flood depths ranging from the knee to neck are considered to have medium hazard levels, and those covered with floods that are higher than the neck have high hazard levels. However, since the flow velocity is also considered, areas that have shallow but fast-flowing flood waters may have a higher hazard level than that denoted by the height of the flood covering it.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:19" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A125" s="8" t="s">
         <v>99</v>
       </c>
@@ -10359,7 +10355,7 @@
 &lt;strong&gt;Flood extent source&lt;/strong&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A126" s="8" t="s">
         <v>99</v>
       </c>
@@ -10423,7 +10419,7 @@
         <v>"UGA": {"drought": "This layer shows the exposed population. It is visualised in shaed of purple on the map when triggered. the number of people exposed is calculated by the population living within a triggered district. The number of people data is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A127" s="8" t="s">
         <v>99</v>
       </c>
@@ -10489,7 +10485,7 @@
         <v>"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012].",</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:19" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A128" s="8" t="s">
         <v>99</v>
       </c>
@@ -10557,7 +10553,7 @@
         <v>"heavy-rain": "&lt;p&gt;Number of people exposed is calculated by the population living in the triggered area.&lt;/p&gt;&lt;br&gt;&lt;p&gt;&lt;strong&gt;Source (Population Data)&lt;/strong&gt;: High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A129" s="8" t="s">
         <v>99</v>
       </c>
@@ -10621,7 +10617,7 @@
         <v>"ZMB": {"drought": "Number of people exposed is calculated by the population living within the districts currently triggered. The number of people data is derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A130" s="8" t="s">
         <v>99</v>
       </c>
@@ -10685,7 +10681,7 @@
         <v>"floods": "Number of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:19" ht="306" x14ac:dyDescent="0.4">
       <c r="A131" s="8" t="s">
         <v>99</v>
       </c>
@@ -10755,7 +10751,7 @@
         <v>"ZWE": {"drought": "&lt;p&gt;Number of people exposed is calculated by the population living in the droughts alert threshold reached area within the district currently triggered. The number of people and the drought extent is derived from the below sources.&lt;/p&gt; &lt;p&gt;Source links:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Population Data: Worldpop &lt;a target='_blank' href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Drought alert threshold reached: ENSO: Seasonal ERSSTv5 (1991-2020 base period) 3-month running average in Ni&amp;ntilde;o 3.4 (5oNorth-5oSouth) (170-120oWest)). &lt;a target='_blank' href='https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt'&gt;https://www.cpc.ncep.noaa.gov/data/indices/3mth.nino34.91-20.ascii.txt&lt;/a&gt; and CHIRPS: Rainfall Estimates from Rain Gauge and Satellite Observations | Climate Hazards Center - UC Santa Barbara (&lt;a target='_blank' href='https://www.chc.ucsb.edu/data/chirps'&gt;https://www.chc.ucsb.edu/data/chirps&lt;/a&gt;)&amp;nbsp;&lt;/li&gt;&lt;li&gt;Crop Yield data: Izumi, Toshichika (2019): Global dataset of historical yields v1.2 and v1.3 aligned version. PANGAEA, &lt;a target='_blank' href='https://doi.org/10.1594/PANGAEA.909132'&gt;https://doi.org/10.1594/PANGAEA.909132&lt;/a&gt;,Supplement to Iizumi, Toshichika; Sakai, T (2020): The global dataset of historical yields for major crops 1981&amp;ndash;2016. Scientific Data, 7(1), &lt;a target='_blank' href='https://doi.org/10.1038/s41597-020-0433-7'&gt;https://doi.org/10.1038/s41597-020-0433-7&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:19" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A132" s="8" t="s">
         <v>99</v>
       </c>
@@ -10821,7 +10817,7 @@
         <v>"population_affected_percentage": {"EGY": {"heavy-rain": "Percentage of people exposed is calculated by the population living in the rainfall extent area within the governorates currently triggered. The number of people and the rainfall extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source Rainfall Extent: Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."},</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A133" s="8" t="s">
         <v>99</v>
       </c>
@@ -10887,7 +10883,7 @@
         <v>"ETH": {"drought": "Percentage of people exposed is calculated by the population living in within the districts currently triggered. The number of people was derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A134" s="8" t="s">
         <v>99</v>
       </c>
@@ -10951,7 +10947,7 @@
         <v>"floods": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:19" ht="247.75" x14ac:dyDescent="0.4">
       <c r="A135" s="8" t="s">
         <v>99</v>
       </c>
@@ -11031,7 +11027,7 @@
 &lt;/ul&gt;"},</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:19" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A136" s="8" t="s">
         <v>99</v>
       </c>
@@ -11107,7 +11103,7 @@
 &lt;/ul&gt;"},</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:19" ht="218.6" x14ac:dyDescent="0.4">
       <c r="A137" s="8" t="s">
         <v>99</v>
       </c>
@@ -11175,7 +11171,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Source (Population Data): High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Source Flood Extent: The flood extent maps are generated by the National Operational Assesment of Hazards(NOAH) project.&lt;a target='_blank' href='https://noah.up.edu.ph/'&gt;https://noah.up.edu.ph/&lt;/a&gt; The 25-year rain return flood hazard maps show low, medium, and high flood hazards represented as yellow, orange, and red respectively. Flood hazards consider take both the height and velocity of the water into consideration and calculates the hazard levels based on the danger they pose to people and structures. Generally, for an average Filipino with a height of 5’ 6”, areas with flood depths from the knee down can be considered to have low hazard levels. Those with flood depths ranging from the knee to neck are considered to have medium hazard levels, and those covered with floods that are higher than the neck have high hazard levels. However, since the flow velocity is also considered, areas that have shallow but fast-flowing flood waters may have a higher hazard level than that denoted by the height of the flood covering it.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:19" ht="262.3" x14ac:dyDescent="0.4">
       <c r="A138" s="8" t="s">
         <v>99</v>
       </c>
@@ -11245,7 +11241,7 @@
 &lt;strong&gt;Flood extent source&lt;/strong&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A139" s="8" t="s">
         <v>99</v>
       </c>
@@ -11311,7 +11307,7 @@
         <v>"UGA": {"floods": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A140" s="8" t="s">
         <v>99</v>
       </c>
@@ -11375,7 +11371,7 @@
         <v>"ZMB": {"floods": "Percentage of people exposed is calculated by the population living in the flood extent area within the districts currently triggered. The number of people and the flood extent are derived from the below sources.&lt;br /&gt;&lt;br /&gt;Source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Source Flood Extent&lt;/b&gt;: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."}},</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A141" s="8" t="s">
         <v>99</v>
       </c>
@@ -11441,7 +11437,7 @@
         <v>"population_over65": {"PHL": {"dengue": "Percentage of people over 65 years of age. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a target='_blank' href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A142" s="8" t="s">
         <v>99</v>
       </c>
@@ -11507,7 +11503,7 @@
         <v>"UGA": {"floods": "Percentage of people over 65 years old.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a target='_blank' href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."}},</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A143" s="8" t="s">
         <v>99</v>
       </c>
@@ -11573,7 +11569,7 @@
         <v>"population_u5": {"ETH": {"drought": "Under age: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a target='_blank' href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A144" s="8" t="s">
         <v>99</v>
       </c>
@@ -11639,7 +11635,7 @@
         <v>"floods": "Under age: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a target='_blank' href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A145" s="8" t="s">
         <v>99</v>
       </c>
@@ -11703,7 +11699,7 @@
         <v>"malaria": "Under age: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a target='_blank' href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A146" s="8" t="s">
         <v>99</v>
       </c>
@@ -11769,7 +11765,7 @@
         <v>"population_u8": {"UGA": {"floods": "Percentage of people under 8 years old.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a target='_blank' href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."}},</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A147" s="8" t="s">
         <v>99</v>
       </c>
@@ -11835,7 +11831,7 @@
         <v>"population_u9": {"PHL": {"dengue": "Percentage of people under 9 years of age. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a target='_blank' href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A148" s="8" t="s">
         <v>99</v>
       </c>
@@ -11899,7 +11895,7 @@
         <v>"populationTotal": {"EGY": {"heavy-rain": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A149" s="8" t="s">
         <v>99</v>
       </c>
@@ -11965,7 +11961,7 @@
         <v>"ETH": {"drought": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A150" s="8" t="s">
         <v>99</v>
       </c>
@@ -12029,7 +12025,7 @@
         <v>"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A151" s="8" t="s">
         <v>99</v>
       </c>
@@ -12093,7 +12089,7 @@
         <v>"malaria": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A152" s="8" t="s">
         <v>99</v>
       </c>
@@ -12165,7 +12161,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A153" s="8" t="s">
         <v>99</v>
       </c>
@@ -12237,7 +12233,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:19" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A154" s="8" t="s">
         <v>99</v>
       </c>
@@ -12305,7 +12301,7 @@
 &lt;p&gt;&lt;strong&gt;Source link:&lt;/strong&gt; peanutButter: An R package to produce rapid-response gridded population estimates from building footprints, version 1.0.0 version 1.0.0. Accessed 15-08-2022. WorldPop, University of Southampton. 2021. &amp;nbsp;&lt;a target='_blank' href='https://apps.worldpop.org/peanutButter/'&gt;https://apps.worldpop.org/peanutButter/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A155" s="8" t="s">
         <v>99</v>
       </c>
@@ -12373,7 +12369,7 @@
 &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:19" ht="174.9" x14ac:dyDescent="0.4">
       <c r="A156" s="8" t="s">
         <v>99</v>
       </c>
@@ -12439,7 +12435,7 @@
         <v>"SSD": {"floods": "This layer shows the total population in the triggered areas, It is visualised in shades of purple that are represented in the legend on the bottom left corner of the map when the layer is selected.The population data is aggregated from the administrative areas.&lt;br&gt;&lt;br&gt; &lt;strong&gt;Population data source&lt;/strong&gt;: WorldPop (&lt;a target='_blank' href='www.worldpop.org'&gt;www.worldpop.org&lt;/a&gt; - School of Geography and Environmental Science, University of Southampton; Department of Geography and Geosciences, University of Louisville; Departement de Geographie, Universite de Namur) and Center for International Earth Science Information Network (CIESIN), Columbia University (2018)."},</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A157" s="8" t="s">
         <v>99</v>
       </c>
@@ -12507,7 +12503,7 @@
 &lt;p&gt;&lt;strong&gt;Population source:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A158" s="8" t="s">
         <v>99</v>
       </c>
@@ -12573,7 +12569,7 @@
         <v>"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A159" s="8" t="s">
         <v>99</v>
       </c>
@@ -12639,7 +12635,7 @@
 &lt;p&gt;&lt;strong&gt;Population source:&lt;/strong&gt; High-Resolution Settlement Layer (HRSL). Source imagery for HRSL &amp;copy; 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. &amp;nbsp;&lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A160" s="8" t="s">
         <v>99</v>
       </c>
@@ -12703,7 +12699,7 @@
         <v>"ZMB": {"drought": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A161" s="8" t="s">
         <v>99</v>
       </c>
@@ -12767,7 +12763,7 @@
         <v>"floods": "Population data is aggregated per administrative area, from the following original source (Population Data): High Resolution Settlement Layer (HRSL). Source imagery for HRSL © 2016 DigitalGlobe. Accessed 01-01-2020. Facebook Connectivity Lab and Center for International Earth Science Information Network - CIESIN - Columbia University. 2016.  &lt;a target='_blank' href='https://www.ciesin.columbia.edu/data/hrsl/'&gt;https://www.ciesin.columbia.edu/data/hrsl/&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:19" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A162" s="8" t="s">
         <v>99</v>
       </c>
@@ -12837,7 +12833,7 @@
         <v>"ZWE": {"drought": "Population data is aggregated per administrative area, from the following original source: Worldpop data:&lt;ul&gt;&lt;li&gt;&lt;a target='_blank' href='https://www.worldpop.org/'&gt;https://www.worldpop.org/&lt;/a&gt;Estimates of total number of people per grid square broken down by gender and age groupings.&lt;/li&gt;&lt;li&gt;Accessed 07-2020 The mapping approach is Pezzulo, C. et al. Sub-national mapping of population pyramids and dependency ratios in Africa and Asia. Sci. Data 4:170089 doi:10.1038/sdata.2017.89 (2017)&lt;/li&gt;&lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A163" s="8" t="s">
         <v>99</v>
       </c>
@@ -12903,7 +12899,7 @@
         <v>"potential_cases": {"ETH": {"malaria": "Potential number of cases are calculated with the assumtion of a rough proportionality between malaria mosquito enviromental suitability and malaria risk. Then estimating a time lag between optimal malaria mosquito environmental conditions and the peak in number of malaria cases."},</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A164" s="8" t="s">
         <v>99</v>
       </c>
@@ -12969,7 +12965,7 @@
         <v>"PHL": {"dengue": "Number of potential dengue cases, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a target='_blank' href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A165" s="8" t="s">
         <v>99</v>
       </c>
@@ -13035,7 +13031,7 @@
         <v>"potential_cases_65": {"ETH": {"malaria": "Elderly: vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates &lt;a target='_blank' href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A166" s="8" t="s">
         <v>99</v>
       </c>
@@ -13101,7 +13097,7 @@
         <v>"PHL": {"dengue": "Number of potential dengue cases among people above 65 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a target='_blank' href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A167" s="8" t="s">
         <v>99</v>
       </c>
@@ -13167,7 +13163,7 @@
         <v>"potential_cases_U5": {"ETH": {"malaria": "Potential cases under 5. Vulnerable population group Ethiopia: High Resolution Population Density Maps + Demographic Estimates.&lt;br /&gt;&lt;br /&gt;Source Data: &lt;a target='_blank' href='https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates'&gt;https://data.humdata.org/dataset/ethiopia-high-resolution-population-density-maps-demographic-estimates&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A168" s="8" t="s">
         <v>99</v>
       </c>
@@ -13233,7 +13229,7 @@
         <v>"potential_cases_U9": {"PHL": {"dengue": "Number of potential dengue cases among children under 9 years of age, based on dengue risk and demographic data. &lt;br /&gt;&lt;br /&gt;Source demographic data: &lt;a target='_blank' href='https://data.humdata.org/dataset/philippines-pre-disaster-indicators'&gt;https://data.humdata.org/dataset/philippines-pre-disaster-indicators/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A169" s="8" t="s">
         <v>99</v>
       </c>
@@ -13299,7 +13295,7 @@
         <v>"poverty_incidence": {"UGA": {"floods": "Poverty Incidence is defined by the Multidiemensional Poverty Index and a $2 a day threshold. The layer gives an estimate of people living in poverty.&lt;br /&gt;&lt;br /&gt;Source: Tatem AJ, Gething PW, Bhatt S, Weiss D and Pezzulo C (2013) Pilot high resolution poverty maps, University of Southampton/Oxford. DOI: 10.5258/SOTON/WP00285. Year: 2010"}},</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A170" s="8" t="s">
         <v>99</v>
       </c>
@@ -13365,7 +13361,7 @@
         <v>"prob_within_50km": {"PHL": {"typhoon": "&lt;p&gt;Probability for a Municipality being with in 50km of the forecasted typhoon track. Source for Typhoon forecast is ECMWF&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A171" s="8" t="s">
         <v>99</v>
       </c>
@@ -13431,7 +13427,7 @@
         <v>"rainfall": {"PHL": {"typhoon": "&lt;p&gt;24 Hour Precipitation Total extracted from forecast issued by The Weather Prediction Center (WPC) of National Atmospheric Administration, NOAA.&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A172" s="8" t="s">
         <v>99</v>
       </c>
@@ -13497,7 +13493,7 @@
         <v>"rainfall_extent": {"EGY": {"heavy-rain": "Global Ensemble Forecast System (GEFS) is a global weather forecast model produced by the NOAA's National Centers for Environmental Prediction (NCEP). Dozens of atmospheric forecast variables up to 16 days in the future, including precipitation, are available through this dataset.&lt;br&gt;&lt;br&gt;The Rainfall Extent layer shows areas where forecasted GEFS precipitation occurrence exceeds defined thresholds."},</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A173" s="8" t="s">
         <v>99</v>
       </c>
@@ -13565,7 +13561,7 @@
         <v>"UGA": {"heavy-rain": "&lt;p&gt;The rainfall extent layer is a dynamic layer that updates every time the model runs (once a day).&lt;br&gt;It’s visualised as squares on the map in a gradient of yellow (low) to red (high) depending on the intensity.&lt;/p&gt;&lt;p&gt;The layer shows the amount of forecasted 1-day cumulative precipitation over the area of interest.&lt;/p&gt;&lt;p&gt;The rainfall forecast is sourced from the European Centre for Medium-Range Weather Forecasts (ECMWF) through the Norwegian Meteorological Institute API (METNO).&lt;br&gt;This is a global model that provides weather forecasts up to 3 days in advance, with a granularity of 1 hour.&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A174" s="8" t="s">
         <v>99</v>
       </c>
@@ -13631,7 +13627,7 @@
         <v>"rainfall_forecast": {"ETH": {"drought": "The rainfall map layer indicates the seasonal forecasting rainfall data for the floods within a return period depending on the EAP (for example 20-years) based on a global hydrological model.&lt;br /&gt;&lt;br /&gt;For the legend see &lt;a target='_blank' href='https://www.icpac.net/seasonal-forecast/'&gt;https://www.icpac.net/seasonal-forecast/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt;Source link: The flood extent maps compare six global flood hazard models and one local model. These models are CaMa-UT [Yamazaki D 2011], GLOFRIS [Winsemius H 2013], ECMWF [Pappenberge 2012], JRC [Dottori 2016], SSBN [Sampson 2015], CIMA-UNEP [UNISDR 2015] and local model ATKINS[2012]."},</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A175" s="8" t="s">
         <v>99</v>
       </c>
@@ -13695,7 +13691,7 @@
         <v>"UGA": {"drought": "This layer shows a dynamic rainfall probability forecast for the (first) month of the selected timeline button. It is updated monthly with the model run. It is visualised in yellow (low) to red (high) gradient on the map. The rainfall map layer indicates the probability for below average rainfall based on SEAS5 seasonal forecasting rainfall data from ECMWF.&lt;br /&gt;&lt;br /&gt;For the legend see &lt;a target='_blank' href='https://www.icpac.net/seasonal-forecast/'&gt;https://www.icpac.net/seasonal-forecast/&lt;/a&gt;&lt;br /&gt;&lt;br /&gt; Source link:  &lt;a target='_blank' href='https://www.ecmwf.int/en/forecasts/datasets'&gt;SEAS5 Seasonal Forecasts&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A176" s="8" t="s">
         <v>99</v>
       </c>
@@ -13759,7 +13755,7 @@
         <v>"red_crescent_branches": {"EGY": {"heavy-rain": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Egyptian Red Crescent Society (ERCS). Year: 2020."}},</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A177" s="8" t="s">
         <v>99</v>
       </c>
@@ -13825,7 +13821,7 @@
         <v>"red_cross_branches": {"EGY": {"heavy-rain": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Egyptian Red Crescent Society (ERCS). Year: 2020."},</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A178" s="8" t="s">
         <v>99</v>
       </c>
@@ -13891,7 +13887,7 @@
         <v>"ETH": {"drought": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Ethiopia Red Cross Society (ERCS). Year: 2020.",</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A179" s="8" t="s">
         <v>99</v>
       </c>
@@ -13957,7 +13953,7 @@
         <v>"floods": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Ethiopia Red Cross Society (ERCS). Year: 2020.",</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A180" s="8" t="s">
         <v>99</v>
       </c>
@@ -14021,7 +14017,7 @@
         <v>"malaria": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Ethiopia Red Cross Society (ERCS). Year: 2020."},</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A181" s="8" t="s">
         <v>99</v>
       </c>
@@ -14095,7 +14091,7 @@
 &lt;p&gt;&lt;strong&gt;Latest updated:&lt;/strong&gt; 2020.&lt;/p&gt;",</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A182" s="8" t="s">
         <v>99</v>
       </c>
@@ -14169,7 +14165,7 @@
 &lt;p&gt;&lt;strong&gt;Latest updated:&lt;/strong&gt; 2020.&lt;/p&gt;"},</v>
       </c>
     </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A183" s="8" t="s">
         <v>99</v>
       </c>
@@ -14233,7 +14229,7 @@
         <v>"MWI": {"floods": "Data not available yet"},</v>
       </c>
     </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A184" s="8" t="s">
         <v>99</v>
       </c>
@@ -14299,7 +14295,7 @@
         <v>"PHL": {"dengue": "Data not available yet",</v>
       </c>
     </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A185" s="8" t="s">
         <v>99</v>
       </c>
@@ -14365,7 +14361,7 @@
         <v>"floods": "Data not available yet"},</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A186" s="8" t="s">
         <v>99</v>
       </c>
@@ -14431,7 +14427,7 @@
         <v>"SSD": {"floods": "This layer is not available as the data is not available yet. When available, this layer will show the locations of the South Sudan Red Cross Society branches."},</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A187" s="8" t="s">
         <v>99</v>
       </c>
@@ -14497,7 +14493,7 @@
         <v>"UGA": {"drought": "This layer represents the locations of the local branches. It is visualised as drop pins with a Red Cross icon. The source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Uganda Red Cross Society (URCS). Year: 2020.",</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A188" s="8" t="s">
         <v>99</v>
       </c>
@@ -14563,7 +14559,7 @@
         <v>"floods": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Uganda Red Cross Society (URCS). Year: 2020.",</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A189" s="8" t="s">
         <v>99</v>
       </c>
@@ -14627,7 +14623,7 @@
         <v>"heavy-rain": "This layer represents the locations of the local branches. It is visualised as drop pins with a Red Cross icon. The source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Uganda Red Cross Society (URCS). Year: 2020."},</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A190" s="8" t="s">
         <v>99</v>
       </c>
@@ -14691,7 +14687,7 @@
         <v>"ZMB": {"drought": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Zambia Red Cross Society (ZRCS). Year: 2020.",</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A191" s="8" t="s">
         <v>99</v>
       </c>
@@ -14757,7 +14753,7 @@
         <v>"floods": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link: Zambia Red Cross Society (ZRCS). Year: 2020."},</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A192" s="8" t="s">
         <v>99</v>
       </c>
@@ -14827,7 +14823,7 @@
         <v>"ZWE": {"drought": "This layer represents the locations of the local branches, the source of this data comes from the National Society and may need updating.&lt;br /&gt;&lt;br /&gt;Source link Zimbabwe: ZRCS last updated July 2021 at provincial level."}},</v>
       </c>
     </row>
-    <row r="193" spans="1:19" ht="54.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:19" ht="54.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A193" s="8" t="s">
         <v>99</v>
       </c>
@@ -14899,7 +14895,7 @@
 &lt;a target='_blank' href='https://prism.philrice.gov.ph/dataproducts/'&gt;https://prism.philrice.gov.ph/dataproducts/&lt;/a&gt; This data is based on the Philippine Rice Information System (PRISM) project which primarily aims to establish a nationwide information system on rice that provide information on rice areas and yield at a particular location and time, and information on factors that are affecting the yield. "}},</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="127.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:19" ht="127.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A194" s="8" t="s">
         <v>99</v>
       </c>
@@ -14913,13 +14909,13 @@
         <v>292</v>
       </c>
       <c r="E194" s="20" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="F194" s="22">
         <v>45191</v>
       </c>
       <c r="G194" s="6" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="H194" s="18"/>
       <c r="I194" s="13" t="str">
@@ -14971,7 +14967,7 @@
 &lt;p&gt;Source: Openstreetmap&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="195" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:19" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A195" s="8" t="s">
         <v>99</v>
       </c>
@@ -14985,13 +14981,13 @@
         <v>292</v>
       </c>
       <c r="E195" s="20" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="F195" s="22">
         <v>45191</v>
       </c>
       <c r="G195" s="6" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="H195" s="18"/>
       <c r="I195" s="13" t="str">
@@ -15043,7 +15039,7 @@
 &lt;p&gt;Source: Openstreetmap&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="196" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A196" s="8" t="s">
         <v>99</v>
       </c>
@@ -15109,7 +15105,7 @@
         <v>"roof_type": {"UGA": {"floods": "Not currently available"}},</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:19" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A197" s="8" t="s">
         <v>99</v>
       </c>
@@ -15123,13 +15119,13 @@
         <v>292</v>
       </c>
       <c r="E197" s="20" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="F197" s="22">
         <v>45191</v>
       </c>
       <c r="G197" s="6" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="H197" s="18"/>
       <c r="I197" s="13" t="str">
@@ -15181,7 +15177,7 @@
 &lt;p&gt;Source: Cloud2Street&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:19" ht="204" x14ac:dyDescent="0.4">
       <c r="A198" s="8" t="s">
         <v>99</v>
       </c>
@@ -15261,7 +15257,7 @@
 &lt;a target='_blank' href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;."}},</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:19" ht="233.15" x14ac:dyDescent="0.4">
       <c r="A199" s="8" t="s">
         <v>99</v>
       </c>
@@ -15341,7 +15337,7 @@
 &lt;a target='_blank' href='https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0'&gt;https://fscluster.org/zimbabwe/document/second-round-crop-and-livestock-0&lt;/a&gt;."}},</v>
       </c>
     </row>
-    <row r="200" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A200" s="8" t="s">
         <v>99</v>
       </c>
@@ -15407,7 +15403,7 @@
         <v>"total_houses": {"PHL": {"typhoon": "&lt;p&gt;Total Number of Housing units in each Municipality&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="201" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A201" s="8" t="s">
         <v>99</v>
       </c>
@@ -15473,7 +15469,7 @@
         <v>"total_idps": {"ETH": {"drought": "Total Internally Displaced People (IDPs) DTM Ethiopia National Displacement Report 7_2022",</v>
       </c>
     </row>
-    <row r="202" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A202" s="8" t="s">
         <v>99</v>
       </c>
@@ -15539,7 +15535,7 @@
         <v>"floods": "Total Internally Displaced People (IDPs) DTM Ethiopia National Displacement Report 7_2022",</v>
       </c>
     </row>
-    <row r="203" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A203" s="8" t="s">
         <v>99</v>
       </c>
@@ -15603,7 +15599,7 @@
         <v>"malaria": "Total Internally Displaced People (IDPs) DTM Ethiopia National Displacement Report 7_2022"}},</v>
       </c>
     </row>
-    <row r="204" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A204" s="8" t="s">
         <v>99</v>
       </c>
@@ -15669,7 +15665,7 @@
         <v>"travel_time_cities": {"ETH": {"floods": "Predicted travel time (minutes) to nearest city &lt;a target='_blank' href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="205" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:19" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A205" s="8" t="s">
         <v>99</v>
       </c>
@@ -15733,7 +15729,7 @@
         <v>"malaria": "Predicted travel time (minutes) to nearest city &lt;a target='_blank' href='https://malariaatlas.org/research-project/accessibility-to-healthcare/'&gt;https://malariaatlas.org/research-project/accessibility-to-healthcare/&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="206" spans="1:19" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:19" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A206" s="8" t="s">
         <v>99</v>
       </c>
@@ -15817,7 +15813,7 @@
 &lt;/ul&gt;"}},</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:19" ht="335.15" x14ac:dyDescent="0.4">
       <c r="A207" s="8" t="s">
         <v>99</v>
       </c>
@@ -15907,7 +15903,7 @@
 &lt;p&gt;&lt;strong&gt;Latest updated:&lt;/strong&gt; month, year&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:19" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A208" s="8" t="s">
         <v>99</v>
       </c>
@@ -15971,7 +15967,7 @@
         <v>"vulnerability_index": {"UGA": {"drought": "This layer shows the vulnerability index. It is visualised in shades of grey or purple in the map depending on if there's a trigger. The vulnerability index is a copy of the 'flood vulnerabilty index' used in the IBF Floods portal. It is a composite index for the context of exposure to the hazard and the capacity to anticipate, cope with and recover from the impacts. The National Society and Technical Working group selected the following criteria below: (including their weight in the total score)&lt;ul&gt;&lt;li&gt;20% Poverty: Poverty incidence&lt;/li&gt;&lt;li&gt;20% Gender: Female-headed household&lt;/li&gt;&lt;li&gt;10% Age: Population below 8-years&lt;/li&gt;&lt;li&gt;10% Age: population 65+,&lt;/li&gt;&lt;li&gt;10 % type of construction: permanent wall type&lt;/li&gt;&lt;li&gt;10 %type of construction: permanent roof type&lt;/li&gt;&lt;li&gt;20% Refugees legal status #of displaced person&lt;/li&gt;&lt;/ul&gt;&lt;br&gt;For further information please refer to the EAP. For sources of the components, see the source layers in the IBF floods portal."}},</v>
       </c>
     </row>
-    <row r="209" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:19" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A209" s="8" t="s">
         <v>99</v>
       </c>
@@ -16045,7 +16041,7 @@
 Ongoing (updated regularly)",</v>
       </c>
     </row>
-    <row r="210" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A210" s="8" t="s">
         <v>99</v>
       </c>
@@ -16115,7 +16111,7 @@
 DSWD, NATIONAL HOUSEHOLD TARGETING OFFICE&lt;/p&gt;"}},</v>
       </c>
     </row>
-    <row r="211" spans="1:19" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A211" s="8" t="s">
         <v>99</v>
       </c>
@@ -16189,7 +16185,7 @@
 Ongoing (updated regularly)",</v>
       </c>
     </row>
-    <row r="212" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A212" s="8" t="s">
         <v>99</v>
       </c>
@@ -16255,7 +16251,7 @@
         <v>"typhoon": "&lt;a target='_blank' href='https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard'&gt;https://data.humdata.org/showcase/philippines-pre-disaster-indicators-dashboard&lt;/a&gt; This dataset has been generated by combining PSGC and 4Ps data from DSWD."}},</v>
       </c>
     </row>
-    <row r="213" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A213" s="8" t="s">
         <v>99</v>
       </c>
@@ -16321,7 +16317,7 @@
         <v>"walking_travel_time_to_health": {"ETH": {"malaria": "Ongoing (updated regularly)"}},</v>
       </c>
     </row>
-    <row r="214" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A214" s="8" t="s">
         <v>99</v>
       </c>
@@ -16387,7 +16383,7 @@
         <v>"wall_type": {"UGA": {"floods": "Percentage of households with permanent wall materials; percentage of buildings with (partly) concrete or brick walls.&lt;br /&gt;&lt;br /&gt;Source link: &lt;a target='_blank' href='https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf'&gt;https://unstats.un.org/unsd/demographic/sources/census/wphc/Uganda/UGA-2016-05-23.pdf.&lt;/a&gt; Year: 2014."}},</v>
       </c>
     </row>
-    <row r="215" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A215" s="8" t="s">
         <v>99</v>
       </c>
@@ -16451,7 +16447,7 @@
         <v>"waterpoints": {"ETH": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a target='_blank' href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A216" s="8" t="s">
         <v>99</v>
       </c>
@@ -16515,7 +16511,7 @@
         <v>"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a target='_blank' href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="217" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A217" s="8" t="s">
         <v>99</v>
       </c>
@@ -16585,7 +16581,7 @@
         <v>"KEN": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a target='_blank' href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="218" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A218" s="8" t="s">
         <v>99</v>
       </c>
@@ -16655,7 +16651,7 @@
         <v>"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source Link: &lt;a target='_blank' href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="219" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A219" s="8" t="s">
         <v>99</v>
       </c>
@@ -16719,7 +16715,7 @@
         <v>"ZMB": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a target='_blank' href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;",</v>
       </c>
     </row>
-    <row r="220" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:19" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A220" s="8" t="s">
         <v>99</v>
       </c>
@@ -16783,7 +16779,7 @@
         <v>"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a target='_blank' href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:19" ht="102" x14ac:dyDescent="0.4">
       <c r="A221" s="8" t="s">
         <v>99</v>
       </c>
@@ -16853,7 +16849,7 @@
         <v>"ZWE": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br /&gt;&lt;br /&gt;Source: &lt;a target='_blank' href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"}},</v>
       </c>
     </row>
-    <row r="222" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A222" s="8" t="s">
         <v>99</v>
       </c>
@@ -16919,7 +16915,7 @@
         <v>"waterpoints_internal": {"MWI": {"flash-floods": "TBD"}},</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:19" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A223" s="8" t="s">
         <v>99</v>
       </c>
@@ -16985,7 +16981,7 @@
         <v>"windspeed": {"PHL": {"typhoon": "&lt;p&gt;Forecasted 1 minute average maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event. The source for this forecast data is ECMWF.&lt;/p&gt;"}}}}</v>
       </c>
     </row>
-    <row r="224" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A224" s="8"/>
       <c r="B224" s="8"/>
       <c r="C224" s="8"/>
@@ -17039,7 +17035,7 @@
         <v/>
       </c>
     </row>
-    <row r="225" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A225" s="8"/>
       <c r="B225" s="8"/>
       <c r="C225" s="8"/>
@@ -17093,7 +17089,7 @@
         <v/>
       </c>
     </row>
-    <row r="226" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A226" s="8"/>
       <c r="B226" s="8"/>
       <c r="C226" s="8"/>
@@ -17147,7 +17143,7 @@
         <v/>
       </c>
     </row>
-    <row r="227" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A227" s="8"/>
       <c r="B227" s="8"/>
       <c r="C227" s="8"/>
@@ -17201,7 +17197,7 @@
         <v/>
       </c>
     </row>
-    <row r="228" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A228" s="8"/>
       <c r="B228" s="8"/>
       <c r="C228" s="8"/>
@@ -17255,7 +17251,7 @@
         <v/>
       </c>
     </row>
-    <row r="229" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A229" s="8"/>
       <c r="B229" s="8"/>
       <c r="C229" s="8"/>
@@ -17309,7 +17305,7 @@
         <v/>
       </c>
     </row>
-    <row r="230" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A230" s="8"/>
       <c r="B230" s="8"/>
       <c r="C230" s="8"/>
@@ -17363,7 +17359,7 @@
         <v/>
       </c>
     </row>
-    <row r="231" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A231" s="8"/>
       <c r="B231" s="8"/>
       <c r="C231" s="8"/>
@@ -17417,7 +17413,7 @@
         <v/>
       </c>
     </row>
-    <row r="232" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A232" s="8"/>
       <c r="B232" s="8"/>
       <c r="C232" s="8"/>
@@ -17471,7 +17467,7 @@
         <v/>
       </c>
     </row>
-    <row r="233" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A233" s="8"/>
       <c r="B233" s="8"/>
       <c r="C233" s="8"/>
@@ -17525,7 +17521,7 @@
         <v/>
       </c>
     </row>
-    <row r="234" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A234" s="8"/>
       <c r="B234" s="8"/>
       <c r="C234" s="8"/>
@@ -17579,7 +17575,7 @@
         <v/>
       </c>
     </row>
-    <row r="235" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A235" s="8"/>
       <c r="B235" s="8"/>
       <c r="C235" s="8"/>
@@ -17633,7 +17629,7 @@
         <v/>
       </c>
     </row>
-    <row r="236" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A236" s="8"/>
       <c r="B236" s="8"/>
       <c r="C236" s="8"/>
@@ -17687,7 +17683,7 @@
         <v/>
       </c>
     </row>
-    <row r="237" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A237" s="8"/>
       <c r="B237" s="8"/>
       <c r="C237" s="8"/>
@@ -17741,7 +17737,7 @@
         <v/>
       </c>
     </row>
-    <row r="238" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A238" s="8"/>
       <c r="B238" s="8"/>
       <c r="C238" s="8"/>
@@ -17795,7 +17791,7 @@
         <v/>
       </c>
     </row>
-    <row r="239" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A239" s="8"/>
       <c r="B239" s="8"/>
       <c r="C239" s="8"/>
@@ -17849,7 +17845,7 @@
         <v/>
       </c>
     </row>
-    <row r="240" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A240" s="8"/>
       <c r="B240" s="8"/>
       <c r="C240" s="8"/>
@@ -17903,7 +17899,7 @@
         <v/>
       </c>
     </row>
-    <row r="241" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A241" s="8"/>
       <c r="B241" s="8"/>
       <c r="C241" s="8"/>
@@ -17957,7 +17953,7 @@
         <v/>
       </c>
     </row>
-    <row r="242" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A242" s="8"/>
       <c r="B242" s="8"/>
       <c r="C242" s="8"/>
@@ -18011,7 +18007,7 @@
         <v/>
       </c>
     </row>
-    <row r="243" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A243" s="8"/>
       <c r="B243" s="8"/>
       <c r="C243" s="8"/>
@@ -18065,7 +18061,7 @@
         <v/>
       </c>
     </row>
-    <row r="244" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A244" s="8"/>
       <c r="B244" s="8"/>
       <c r="C244" s="8"/>
@@ -18119,7 +18115,7 @@
         <v/>
       </c>
     </row>
-    <row r="245" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A245" s="8"/>
       <c r="B245" s="8"/>
       <c r="C245" s="8"/>
@@ -18173,7 +18169,7 @@
         <v/>
       </c>
     </row>
-    <row r="246" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A246" s="8"/>
       <c r="B246" s="8"/>
       <c r="C246" s="8"/>
@@ -18227,7 +18223,7 @@
         <v/>
       </c>
     </row>
-    <row r="247" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A247" s="8"/>
       <c r="B247" s="8"/>
       <c r="C247" s="8"/>
@@ -18281,7 +18277,7 @@
         <v/>
       </c>
     </row>
-    <row r="248" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A248" s="8"/>
       <c r="B248" s="8"/>
       <c r="C248" s="8"/>
@@ -18335,7 +18331,7 @@
         <v/>
       </c>
     </row>
-    <row r="249" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A249" s="8"/>
       <c r="B249" s="8"/>
       <c r="C249" s="8"/>
@@ -18389,7 +18385,7 @@
         <v/>
       </c>
     </row>
-    <row r="250" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A250" s="8"/>
       <c r="B250" s="8"/>
       <c r="C250" s="8"/>
@@ -18443,7 +18439,7 @@
         <v/>
       </c>
     </row>
-    <row r="251" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A251" s="8"/>
       <c r="B251" s="8"/>
       <c r="C251" s="8"/>
@@ -18497,7 +18493,7 @@
         <v/>
       </c>
     </row>
-    <row r="252" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A252" s="8"/>
       <c r="B252" s="8"/>
       <c r="C252" s="8"/>
@@ -18551,7 +18547,7 @@
         <v/>
       </c>
     </row>
-    <row r="253" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A253" s="8"/>
       <c r="B253" s="8"/>
       <c r="C253" s="8"/>
@@ -18605,7 +18601,7 @@
         <v/>
       </c>
     </row>
-    <row r="254" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A254" s="8"/>
       <c r="B254" s="8"/>
       <c r="C254" s="8"/>
@@ -18659,7 +18655,7 @@
         <v/>
       </c>
     </row>
-    <row r="255" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A255" s="8"/>
       <c r="B255" s="8"/>
       <c r="C255" s="8"/>
@@ -18713,7 +18709,7 @@
         <v/>
       </c>
     </row>
-    <row r="256" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A256" s="8"/>
       <c r="B256" s="8"/>
       <c r="C256" s="8"/>
@@ -18767,7 +18763,7 @@
         <v/>
       </c>
     </row>
-    <row r="257" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A257" s="8"/>
       <c r="B257" s="8"/>
       <c r="C257" s="8"/>
@@ -18821,7 +18817,7 @@
         <v/>
       </c>
     </row>
-    <row r="258" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A258" s="8"/>
       <c r="B258" s="8"/>
       <c r="C258" s="8"/>
@@ -18875,7 +18871,7 @@
         <v/>
       </c>
     </row>
-    <row r="259" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A259" s="8"/>
       <c r="B259" s="8"/>
       <c r="C259" s="8"/>
@@ -18929,7 +18925,7 @@
         <v/>
       </c>
     </row>
-    <row r="260" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A260" s="8"/>
       <c r="B260" s="8"/>
       <c r="C260" s="8"/>
@@ -18983,7 +18979,7 @@
         <v/>
       </c>
     </row>
-    <row r="261" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A261" s="8"/>
       <c r="B261" s="8"/>
       <c r="C261" s="8"/>
@@ -19037,7 +19033,7 @@
         <v/>
       </c>
     </row>
-    <row r="262" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A262" s="8"/>
       <c r="B262" s="8"/>
       <c r="C262" s="8"/>
@@ -19091,7 +19087,7 @@
         <v/>
       </c>
     </row>
-    <row r="263" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A263" s="8"/>
       <c r="B263" s="8"/>
       <c r="C263" s="8"/>
@@ -19145,7 +19141,7 @@
         <v/>
       </c>
     </row>
-    <row r="264" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A264" s="8"/>
       <c r="B264" s="8"/>
       <c r="C264" s="8"/>
@@ -19199,7 +19195,7 @@
         <v/>
       </c>
     </row>
-    <row r="265" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A265" s="8"/>
       <c r="B265" s="8"/>
       <c r="C265" s="8"/>
@@ -19253,7 +19249,7 @@
         <v/>
       </c>
     </row>
-    <row r="266" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A266" s="8"/>
       <c r="B266" s="8"/>
       <c r="C266" s="8"/>
@@ -19307,7 +19303,7 @@
         <v/>
       </c>
     </row>
-    <row r="267" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A267" s="8"/>
       <c r="B267" s="8"/>
       <c r="C267" s="8"/>
@@ -19361,7 +19357,7 @@
         <v/>
       </c>
     </row>
-    <row r="268" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A268" s="8"/>
       <c r="B268" s="8"/>
       <c r="C268" s="8"/>
@@ -19415,7 +19411,7 @@
         <v/>
       </c>
     </row>
-    <row r="269" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A269" s="8"/>
       <c r="B269" s="8"/>
       <c r="C269" s="8"/>
@@ -19469,7 +19465,7 @@
         <v/>
       </c>
     </row>
-    <row r="270" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A270" s="8"/>
       <c r="B270" s="8"/>
       <c r="C270" s="8"/>
@@ -19523,7 +19519,7 @@
         <v/>
       </c>
     </row>
-    <row r="271" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A271" s="8"/>
       <c r="B271" s="8"/>
       <c r="C271" s="8"/>
@@ -19577,7 +19573,7 @@
         <v/>
       </c>
     </row>
-    <row r="272" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A272" s="8"/>
       <c r="B272" s="8"/>
       <c r="C272" s="8"/>
@@ -19631,7 +19627,7 @@
         <v/>
       </c>
     </row>
-    <row r="273" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A273" s="8"/>
       <c r="B273" s="8"/>
       <c r="C273" s="8"/>
@@ -19685,7 +19681,7 @@
         <v/>
       </c>
     </row>
-    <row r="274" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A274" s="8"/>
       <c r="B274" s="8"/>
       <c r="C274" s="8"/>
@@ -19739,7 +19735,7 @@
         <v/>
       </c>
     </row>
-    <row r="275" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A275" s="8"/>
       <c r="B275" s="8"/>
       <c r="C275" s="8"/>
@@ -19793,7 +19789,7 @@
         <v/>
       </c>
     </row>
-    <row r="276" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A276" s="8"/>
       <c r="B276" s="8"/>
       <c r="C276" s="8"/>
@@ -19847,7 +19843,7 @@
         <v/>
       </c>
     </row>
-    <row r="277" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A277" s="8"/>
       <c r="B277" s="8"/>
       <c r="C277" s="8"/>
@@ -19901,7 +19897,7 @@
         <v/>
       </c>
     </row>
-    <row r="278" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A278" s="8"/>
       <c r="B278" s="8"/>
       <c r="C278" s="8"/>
@@ -19955,7 +19951,7 @@
         <v/>
       </c>
     </row>
-    <row r="279" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A279" s="8"/>
       <c r="B279" s="8"/>
       <c r="C279" s="8"/>
@@ -20009,7 +20005,7 @@
         <v/>
       </c>
     </row>
-    <row r="280" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A280" s="8"/>
       <c r="B280" s="8"/>
       <c r="C280" s="8"/>
@@ -20063,7 +20059,7 @@
         <v/>
       </c>
     </row>
-    <row r="281" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A281" s="8"/>
       <c r="B281" s="8"/>
       <c r="C281" s="8"/>
@@ -20117,7 +20113,7 @@
         <v/>
       </c>
     </row>
-    <row r="282" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A282" s="8"/>
       <c r="B282" s="8"/>
       <c r="C282" s="8"/>
@@ -20171,7 +20167,7 @@
         <v/>
       </c>
     </row>
-    <row r="283" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A283" s="8"/>
       <c r="B283" s="8"/>
       <c r="C283" s="8"/>
@@ -20225,7 +20221,7 @@
         <v/>
       </c>
     </row>
-    <row r="284" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A284" s="8"/>
       <c r="B284" s="8"/>
       <c r="C284" s="8"/>
@@ -20279,7 +20275,7 @@
         <v/>
       </c>
     </row>
-    <row r="285" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A285" s="8"/>
       <c r="B285" s="8"/>
       <c r="C285" s="8"/>
@@ -20333,7 +20329,7 @@
         <v/>
       </c>
     </row>
-    <row r="286" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A286" s="8"/>
       <c r="B286" s="8"/>
       <c r="C286" s="8"/>
@@ -20387,7 +20383,7 @@
         <v/>
       </c>
     </row>
-    <row r="287" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A287" s="8"/>
       <c r="B287" s="8"/>
       <c r="C287" s="8"/>
@@ -20441,7 +20437,7 @@
         <v/>
       </c>
     </row>
-    <row r="288" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A288" s="8"/>
       <c r="B288" s="8"/>
       <c r="C288" s="8"/>
@@ -20495,7 +20491,7 @@
         <v/>
       </c>
     </row>
-    <row r="289" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A289" s="8"/>
       <c r="B289" s="8"/>
       <c r="C289" s="8"/>
@@ -20549,7 +20545,7 @@
         <v/>
       </c>
     </row>
-    <row r="290" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A290" s="8"/>
       <c r="B290" s="8"/>
       <c r="C290" s="8"/>
@@ -20603,7 +20599,7 @@
         <v/>
       </c>
     </row>
-    <row r="291" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A291" s="8"/>
       <c r="B291" s="8"/>
       <c r="C291" s="8"/>
@@ -20657,7 +20653,7 @@
         <v/>
       </c>
     </row>
-    <row r="292" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A292" s="8"/>
       <c r="B292" s="8"/>
       <c r="C292" s="8"/>
@@ -20711,7 +20707,7 @@
         <v/>
       </c>
     </row>
-    <row r="293" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A293" s="8"/>
       <c r="B293" s="8"/>
       <c r="C293" s="8"/>
@@ -20765,7 +20761,7 @@
         <v/>
       </c>
     </row>
-    <row r="294" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A294" s="8"/>
       <c r="B294" s="8"/>
       <c r="C294" s="8"/>
@@ -20819,7 +20815,7 @@
         <v/>
       </c>
     </row>
-    <row r="295" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A295" s="8"/>
       <c r="B295" s="8"/>
       <c r="C295" s="8"/>
@@ -20873,7 +20869,7 @@
         <v/>
       </c>
     </row>
-    <row r="296" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A296" s="8"/>
       <c r="B296" s="8"/>
       <c r="C296" s="8"/>
@@ -20927,7 +20923,7 @@
         <v/>
       </c>
     </row>
-    <row r="297" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A297" s="8"/>
       <c r="B297" s="8"/>
       <c r="C297" s="8"/>
@@ -20981,7 +20977,7 @@
         <v/>
       </c>
     </row>
-    <row r="298" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A298" s="8"/>
       <c r="B298" s="8"/>
       <c r="C298" s="8"/>
@@ -21035,7 +21031,7 @@
         <v/>
       </c>
     </row>
-    <row r="299" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A299" s="8"/>
       <c r="B299" s="8"/>
       <c r="C299" s="8"/>
@@ -21089,7 +21085,7 @@
         <v/>
       </c>
     </row>
-    <row r="300" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A300" s="8"/>
       <c r="B300" s="8"/>
       <c r="C300" s="8"/>
@@ -21143,7 +21139,7 @@
         <v/>
       </c>
     </row>
-    <row r="301" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A301" s="8"/>
       <c r="B301" s="8"/>
       <c r="C301" s="8"/>
@@ -21197,7 +21193,7 @@
         <v/>
       </c>
     </row>
-    <row r="302" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A302" s="8"/>
       <c r="B302" s="8"/>
       <c r="C302" s="8"/>
@@ -21251,7 +21247,7 @@
         <v/>
       </c>
     </row>
-    <row r="303" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A303" s="8"/>
       <c r="B303" s="8"/>
       <c r="C303" s="8"/>
@@ -21305,7 +21301,7 @@
         <v/>
       </c>
     </row>
-    <row r="304" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A304" s="8"/>
       <c r="B304" s="8"/>
       <c r="C304" s="8"/>
@@ -21359,7 +21355,7 @@
         <v/>
       </c>
     </row>
-    <row r="305" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A305" s="8"/>
       <c r="B305" s="8"/>
       <c r="C305" s="8"/>
@@ -21413,7 +21409,7 @@
         <v/>
       </c>
     </row>
-    <row r="306" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A306" s="8"/>
       <c r="B306" s="8"/>
       <c r="C306" s="8"/>
@@ -21467,7 +21463,7 @@
         <v/>
       </c>
     </row>
-    <row r="307" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A307" s="8"/>
       <c r="B307" s="8"/>
       <c r="C307" s="8"/>
@@ -21521,7 +21517,7 @@
         <v/>
       </c>
     </row>
-    <row r="308" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A308" s="8"/>
       <c r="B308" s="8"/>
       <c r="C308" s="8"/>
@@ -21575,7 +21571,7 @@
         <v/>
       </c>
     </row>
-    <row r="309" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A309" s="8"/>
       <c r="B309" s="8"/>
       <c r="C309" s="8"/>
@@ -21629,7 +21625,7 @@
         <v/>
       </c>
     </row>
-    <row r="310" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A310" s="8"/>
       <c r="B310" s="8"/>
       <c r="C310" s="8"/>
@@ -21683,7 +21679,7 @@
         <v/>
       </c>
     </row>
-    <row r="311" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A311" s="8"/>
       <c r="B311" s="8"/>
       <c r="C311" s="8"/>
@@ -21737,7 +21733,7 @@
         <v/>
       </c>
     </row>
-    <row r="312" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A312" s="8"/>
       <c r="B312" s="8"/>
       <c r="C312" s="8"/>
@@ -21791,7 +21787,7 @@
         <v/>
       </c>
     </row>
-    <row r="313" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A313" s="8"/>
       <c r="B313" s="8"/>
       <c r="C313" s="8"/>
@@ -21845,7 +21841,7 @@
         <v/>
       </c>
     </row>
-    <row r="314" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A314" s="8"/>
       <c r="B314" s="8"/>
       <c r="C314" s="8"/>
@@ -21899,7 +21895,7 @@
         <v/>
       </c>
     </row>
-    <row r="315" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A315" s="8"/>
       <c r="B315" s="8"/>
       <c r="C315" s="8"/>
@@ -21953,7 +21949,7 @@
         <v/>
       </c>
     </row>
-    <row r="316" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A316" s="8"/>
       <c r="B316" s="8"/>
       <c r="C316" s="8"/>
@@ -22007,7 +22003,7 @@
         <v/>
       </c>
     </row>
-    <row r="317" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A317" s="8"/>
       <c r="B317" s="8"/>
       <c r="C317" s="8"/>
@@ -22061,7 +22057,7 @@
         <v/>
       </c>
     </row>
-    <row r="318" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A318" s="8"/>
       <c r="B318" s="8"/>
       <c r="C318" s="8"/>
@@ -22115,7 +22111,7 @@
         <v/>
       </c>
     </row>
-    <row r="319" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A319" s="8"/>
       <c r="B319" s="8"/>
       <c r="C319" s="8"/>
@@ -22169,7 +22165,7 @@
         <v/>
       </c>
     </row>
-    <row r="320" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A320" s="8"/>
       <c r="B320" s="8"/>
       <c r="C320" s="8"/>
@@ -22223,7 +22219,7 @@
         <v/>
       </c>
     </row>
-    <row r="321" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A321" s="8"/>
       <c r="B321" s="8"/>
       <c r="C321" s="8"/>
@@ -22277,7 +22273,7 @@
         <v/>
       </c>
     </row>
-    <row r="322" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A322" s="8"/>
       <c r="B322" s="8"/>
       <c r="C322" s="8"/>
@@ -22331,7 +22327,7 @@
         <v/>
       </c>
     </row>
-    <row r="323" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A323" s="8"/>
       <c r="B323" s="8"/>
       <c r="C323" s="8"/>
@@ -22385,7 +22381,7 @@
         <v/>
       </c>
     </row>
-    <row r="324" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A324" s="8"/>
       <c r="B324" s="8"/>
       <c r="C324" s="8"/>
@@ -22439,7 +22435,7 @@
         <v/>
       </c>
     </row>
-    <row r="325" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A325" s="8"/>
       <c r="B325" s="8"/>
       <c r="C325" s="8"/>
@@ -22493,7 +22489,7 @@
         <v/>
       </c>
     </row>
-    <row r="326" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A326" s="8"/>
       <c r="B326" s="8"/>
       <c r="C326" s="8"/>
@@ -22547,7 +22543,7 @@
         <v/>
       </c>
     </row>
-    <row r="327" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A327" s="8"/>
       <c r="B327" s="8"/>
       <c r="C327" s="8"/>
@@ -22601,7 +22597,7 @@
         <v/>
       </c>
     </row>
-    <row r="328" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A328" s="8"/>
       <c r="B328" s="8"/>
       <c r="C328" s="8"/>
@@ -22655,7 +22651,7 @@
         <v/>
       </c>
     </row>
-    <row r="329" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A329" s="8"/>
       <c r="B329" s="8"/>
       <c r="C329" s="8"/>
@@ -22709,7 +22705,7 @@
         <v/>
       </c>
     </row>
-    <row r="330" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A330" s="8"/>
       <c r="B330" s="8"/>
       <c r="C330" s="8"/>
@@ -22763,7 +22759,7 @@
         <v/>
       </c>
     </row>
-    <row r="331" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A331" s="8"/>
       <c r="B331" s="8"/>
       <c r="C331" s="8"/>
@@ -22817,7 +22813,7 @@
         <v/>
       </c>
     </row>
-    <row r="332" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A332" s="8"/>
       <c r="B332" s="8"/>
       <c r="C332" s="8"/>
@@ -22871,7 +22867,7 @@
         <v/>
       </c>
     </row>
-    <row r="333" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A333" s="8"/>
       <c r="B333" s="8"/>
       <c r="C333" s="8"/>
@@ -22925,7 +22921,7 @@
         <v/>
       </c>
     </row>
-    <row r="334" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A334" s="8"/>
       <c r="B334" s="8"/>
       <c r="C334" s="8"/>
@@ -22979,7 +22975,7 @@
         <v/>
       </c>
     </row>
-    <row r="335" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A335" s="8"/>
       <c r="B335" s="8"/>
       <c r="C335" s="8"/>
@@ -23033,7 +23029,7 @@
         <v/>
       </c>
     </row>
-    <row r="336" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A336" s="8"/>
       <c r="B336" s="8"/>
       <c r="C336" s="8"/>
@@ -23087,7 +23083,7 @@
         <v/>
       </c>
     </row>
-    <row r="337" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A337" s="8"/>
       <c r="B337" s="8"/>
       <c r="C337" s="8"/>
@@ -23141,7 +23137,7 @@
         <v/>
       </c>
     </row>
-    <row r="338" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A338" s="8"/>
       <c r="B338" s="8"/>
       <c r="C338" s="8"/>
@@ -23195,7 +23191,7 @@
         <v/>
       </c>
     </row>
-    <row r="339" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="339" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A339" s="8"/>
       <c r="B339" s="8"/>
       <c r="C339" s="8"/>
@@ -23249,7 +23245,7 @@
         <v/>
       </c>
     </row>
-    <row r="340" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A340" s="8"/>
       <c r="B340" s="8"/>
       <c r="C340" s="8"/>
@@ -23303,7 +23299,7 @@
         <v/>
       </c>
     </row>
-    <row r="341" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A341" s="8"/>
       <c r="B341" s="8"/>
       <c r="C341" s="8"/>
@@ -23357,7 +23353,7 @@
         <v/>
       </c>
     </row>
-    <row r="342" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A342" s="8"/>
       <c r="B342" s="8"/>
       <c r="C342" s="8"/>
@@ -23411,7 +23407,7 @@
         <v/>
       </c>
     </row>
-    <row r="343" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A343" s="8"/>
       <c r="B343" s="8"/>
       <c r="C343" s="8"/>
@@ -23465,7 +23461,7 @@
         <v/>
       </c>
     </row>
-    <row r="344" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A344" s="8"/>
       <c r="B344" s="8"/>
       <c r="C344" s="8"/>
@@ -23519,7 +23515,7 @@
         <v/>
       </c>
     </row>
-    <row r="345" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A345" s="8"/>
       <c r="B345" s="8"/>
       <c r="C345" s="8"/>
@@ -23573,7 +23569,7 @@
         <v/>
       </c>
     </row>
-    <row r="346" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A346" s="8"/>
       <c r="B346" s="8"/>
       <c r="C346" s="8"/>
@@ -23627,7 +23623,7 @@
         <v/>
       </c>
     </row>
-    <row r="347" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="347" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A347" s="8"/>
       <c r="B347" s="8"/>
       <c r="C347" s="8"/>
@@ -23681,7 +23677,7 @@
         <v/>
       </c>
     </row>
-    <row r="348" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A348" s="8"/>
       <c r="B348" s="8"/>
       <c r="C348" s="8"/>
@@ -23735,7 +23731,7 @@
         <v/>
       </c>
     </row>
-    <row r="349" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A349" s="8"/>
       <c r="B349" s="8"/>
       <c r="C349" s="8"/>
@@ -23789,7 +23785,7 @@
         <v/>
       </c>
     </row>
-    <row r="350" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A350" s="8"/>
       <c r="B350" s="8"/>
       <c r="C350" s="8"/>
@@ -23843,7 +23839,7 @@
         <v/>
       </c>
     </row>
-    <row r="351" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A351" s="8"/>
       <c r="B351" s="8"/>
       <c r="C351" s="8"/>
@@ -23897,7 +23893,7 @@
         <v/>
       </c>
     </row>
-    <row r="352" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A352" s="8"/>
       <c r="B352" s="8"/>
       <c r="C352" s="8"/>
@@ -23951,7 +23947,7 @@
         <v/>
       </c>
     </row>
-    <row r="353" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="353" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A353" s="8"/>
       <c r="B353" s="8"/>
       <c r="C353" s="8"/>
@@ -24005,7 +24001,7 @@
         <v/>
       </c>
     </row>
-    <row r="354" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A354" s="8"/>
       <c r="B354" s="8"/>
       <c r="C354" s="8"/>
@@ -24059,7 +24055,7 @@
         <v/>
       </c>
     </row>
-    <row r="355" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A355" s="8"/>
       <c r="B355" s="8"/>
       <c r="C355" s="8"/>
@@ -24113,7 +24109,7 @@
         <v/>
       </c>
     </row>
-    <row r="356" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A356" s="8"/>
       <c r="B356" s="8"/>
       <c r="C356" s="8"/>
@@ -24167,7 +24163,7 @@
         <v/>
       </c>
     </row>
-    <row r="357" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A357" s="8"/>
       <c r="B357" s="8"/>
       <c r="C357" s="8"/>
@@ -24221,7 +24217,7 @@
         <v/>
       </c>
     </row>
-    <row r="358" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A358" s="8"/>
       <c r="B358" s="8"/>
       <c r="C358" s="8"/>
@@ -24275,7 +24271,7 @@
         <v/>
       </c>
     </row>
-    <row r="359" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A359" s="8"/>
       <c r="B359" s="8"/>
       <c r="C359" s="8"/>
@@ -24329,7 +24325,7 @@
         <v/>
       </c>
     </row>
-    <row r="360" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A360" s="8"/>
       <c r="B360" s="8"/>
       <c r="C360" s="8"/>
@@ -24383,7 +24379,7 @@
         <v/>
       </c>
     </row>
-    <row r="361" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A361" s="8"/>
       <c r="B361" s="8"/>
       <c r="C361" s="8"/>
@@ -24437,7 +24433,7 @@
         <v/>
       </c>
     </row>
-    <row r="362" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A362" s="8"/>
       <c r="B362" s="8"/>
       <c r="C362" s="8"/>
@@ -24491,7 +24487,7 @@
         <v/>
       </c>
     </row>
-    <row r="363" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A363" s="8"/>
       <c r="B363" s="8"/>
       <c r="C363" s="8"/>
@@ -24545,7 +24541,7 @@
         <v/>
       </c>
     </row>
-    <row r="364" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A364" s="8"/>
       <c r="B364" s="8"/>
       <c r="C364" s="8"/>
@@ -24599,7 +24595,7 @@
         <v/>
       </c>
     </row>
-    <row r="365" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="365" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A365" s="8"/>
       <c r="B365" s="8"/>
       <c r="C365" s="8"/>
@@ -24653,7 +24649,7 @@
         <v/>
       </c>
     </row>
-    <row r="366" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A366" s="8"/>
       <c r="B366" s="8"/>
       <c r="C366" s="8"/>
@@ -24707,7 +24703,7 @@
         <v/>
       </c>
     </row>
-    <row r="367" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A367" s="8"/>
       <c r="B367" s="8"/>
       <c r="C367" s="8"/>
@@ -24761,7 +24757,7 @@
         <v/>
       </c>
     </row>
-    <row r="368" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="368" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A368" s="8"/>
       <c r="B368" s="8"/>
       <c r="C368" s="8"/>
@@ -24815,7 +24811,7 @@
         <v/>
       </c>
     </row>
-    <row r="369" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A369" s="8"/>
       <c r="B369" s="8"/>
       <c r="C369" s="8"/>
@@ -24869,7 +24865,7 @@
         <v/>
       </c>
     </row>
-    <row r="370" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A370" s="8"/>
       <c r="B370" s="8"/>
       <c r="C370" s="8"/>
@@ -24923,7 +24919,7 @@
         <v/>
       </c>
     </row>
-    <row r="371" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="371" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A371" s="8"/>
       <c r="B371" s="8"/>
       <c r="C371" s="8"/>
@@ -24977,7 +24973,7 @@
         <v/>
       </c>
     </row>
-    <row r="372" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A372" s="8"/>
       <c r="B372" s="8"/>
       <c r="C372" s="8"/>
@@ -25031,7 +25027,7 @@
         <v/>
       </c>
     </row>
-    <row r="373" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A373" s="8"/>
       <c r="B373" s="8"/>
       <c r="C373" s="8"/>
@@ -25085,7 +25081,7 @@
         <v/>
       </c>
     </row>
-    <row r="374" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A374" s="8"/>
       <c r="B374" s="8"/>
       <c r="C374" s="8"/>
@@ -25139,7 +25135,7 @@
         <v/>
       </c>
     </row>
-    <row r="375" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="375" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A375" s="8"/>
       <c r="B375" s="8"/>
       <c r="C375" s="8"/>
@@ -25193,7 +25189,7 @@
         <v/>
       </c>
     </row>
-    <row r="376" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A376" s="8"/>
       <c r="B376" s="8"/>
       <c r="C376" s="8"/>
@@ -25247,7 +25243,7 @@
         <v/>
       </c>
     </row>
-    <row r="377" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="377" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A377" s="8"/>
       <c r="B377" s="8"/>
       <c r="C377" s="8"/>
@@ -25301,7 +25297,7 @@
         <v/>
       </c>
     </row>
-    <row r="378" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="378" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A378" s="8"/>
       <c r="B378" s="8"/>
       <c r="C378" s="8"/>
@@ -25355,7 +25351,7 @@
         <v/>
       </c>
     </row>
-    <row r="379" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A379" s="8"/>
       <c r="B379" s="8"/>
       <c r="C379" s="8"/>
@@ -25409,7 +25405,7 @@
         <v/>
       </c>
     </row>
-    <row r="380" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="380" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A380" s="8"/>
       <c r="B380" s="8"/>
       <c r="C380" s="8"/>
@@ -25463,7 +25459,7 @@
         <v/>
       </c>
     </row>
-    <row r="381" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="381" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A381" s="8"/>
       <c r="B381" s="8"/>
       <c r="C381" s="8"/>
@@ -25517,7 +25513,7 @@
         <v/>
       </c>
     </row>
-    <row r="382" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="382" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A382" s="8"/>
       <c r="B382" s="8"/>
       <c r="C382" s="8"/>
@@ -25571,7 +25567,7 @@
         <v/>
       </c>
     </row>
-    <row r="383" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="383" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A383" s="8"/>
       <c r="B383" s="8"/>
       <c r="C383" s="8"/>
@@ -25625,7 +25621,7 @@
         <v/>
       </c>
     </row>
-    <row r="384" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="384" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A384" s="8"/>
       <c r="B384" s="8"/>
       <c r="C384" s="8"/>
@@ -25679,7 +25675,7 @@
         <v/>
       </c>
     </row>
-    <row r="385" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A385" s="8"/>
       <c r="B385" s="8"/>
       <c r="C385" s="8"/>
@@ -25733,7 +25729,7 @@
         <v/>
       </c>
     </row>
-    <row r="386" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="386" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A386" s="8"/>
       <c r="B386" s="8"/>
       <c r="C386" s="8"/>
@@ -25783,11 +25779,11 @@
         <v>}</v>
       </c>
       <c r="S386" s="12" t="str">
-        <f t="shared" ref="S386:S449" si="76">IF(A386="","",I386&amp;J386&amp;K386&amp;L386&amp;M386&amp;N386&amp;O386&amp;P386&amp;Q386&amp;R386)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="387" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="S386:S419" si="76">IF(A386="","",I386&amp;J386&amp;K386&amp;L386&amp;M386&amp;N386&amp;O386&amp;P386&amp;Q386&amp;R386)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="387" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A387" s="8"/>
       <c r="B387" s="8"/>
       <c r="C387" s="8"/>
@@ -25841,7 +25837,7 @@
         <v/>
       </c>
     </row>
-    <row r="388" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="388" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A388" s="8"/>
       <c r="B388" s="8"/>
       <c r="C388" s="8"/>
@@ -25895,7 +25891,7 @@
         <v/>
       </c>
     </row>
-    <row r="389" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="389" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A389" s="8"/>
       <c r="B389" s="8"/>
       <c r="C389" s="8"/>
@@ -25949,7 +25945,7 @@
         <v/>
       </c>
     </row>
-    <row r="390" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="390" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A390" s="8"/>
       <c r="B390" s="8"/>
       <c r="C390" s="8"/>
@@ -26003,7 +25999,7 @@
         <v/>
       </c>
     </row>
-    <row r="391" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="391" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A391" s="8"/>
       <c r="B391" s="8"/>
       <c r="C391" s="8"/>
@@ -26057,7 +26053,7 @@
         <v/>
       </c>
     </row>
-    <row r="392" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="392" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A392" s="8"/>
       <c r="B392" s="8"/>
       <c r="C392" s="8"/>
@@ -26111,7 +26107,7 @@
         <v/>
       </c>
     </row>
-    <row r="393" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="393" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A393" s="8"/>
       <c r="B393" s="8"/>
       <c r="C393" s="8"/>
@@ -26165,7 +26161,7 @@
         <v/>
       </c>
     </row>
-    <row r="394" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="394" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A394" s="8"/>
       <c r="B394" s="8"/>
       <c r="C394" s="8"/>
@@ -26219,7 +26215,7 @@
         <v/>
       </c>
     </row>
-    <row r="395" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="395" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A395" s="8"/>
       <c r="B395" s="8"/>
       <c r="C395" s="8"/>
@@ -26273,7 +26269,7 @@
         <v/>
       </c>
     </row>
-    <row r="396" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="396" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A396" s="8"/>
       <c r="B396" s="8"/>
       <c r="C396" s="8"/>
@@ -26327,7 +26323,7 @@
         <v/>
       </c>
     </row>
-    <row r="397" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="397" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A397" s="8"/>
       <c r="B397" s="8"/>
       <c r="C397" s="8"/>
@@ -26381,7 +26377,7 @@
         <v/>
       </c>
     </row>
-    <row r="398" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="398" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A398" s="8"/>
       <c r="B398" s="8"/>
       <c r="C398" s="8"/>
@@ -26435,7 +26431,7 @@
         <v/>
       </c>
     </row>
-    <row r="399" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="399" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A399" s="8"/>
       <c r="B399" s="8"/>
       <c r="C399" s="8"/>
@@ -26489,7 +26485,7 @@
         <v/>
       </c>
     </row>
-    <row r="400" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="400" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A400" s="8"/>
       <c r="B400" s="8"/>
       <c r="C400" s="8"/>
@@ -26543,7 +26539,7 @@
         <v/>
       </c>
     </row>
-    <row r="401" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="401" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A401" s="8"/>
       <c r="B401" s="8"/>
       <c r="C401" s="8"/>
@@ -26597,7 +26593,7 @@
         <v/>
       </c>
     </row>
-    <row r="402" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="402" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A402" s="8"/>
       <c r="B402" s="8"/>
       <c r="C402" s="8"/>
@@ -26651,7 +26647,7 @@
         <v/>
       </c>
     </row>
-    <row r="403" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="403" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A403" s="8"/>
       <c r="B403" s="8"/>
       <c r="C403" s="8"/>
@@ -26705,7 +26701,7 @@
         <v/>
       </c>
     </row>
-    <row r="404" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="404" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A404" s="8"/>
       <c r="B404" s="8"/>
       <c r="C404" s="8"/>
@@ -26759,7 +26755,7 @@
         <v/>
       </c>
     </row>
-    <row r="405" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="405" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A405" s="8"/>
       <c r="B405" s="8"/>
       <c r="C405" s="8"/>
@@ -26813,7 +26809,7 @@
         <v/>
       </c>
     </row>
-    <row r="406" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="406" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A406" s="8"/>
       <c r="B406" s="8"/>
       <c r="C406" s="8"/>
@@ -26867,7 +26863,7 @@
         <v/>
       </c>
     </row>
-    <row r="407" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="407" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A407" s="8"/>
       <c r="B407" s="8"/>
       <c r="C407" s="8"/>
@@ -26921,7 +26917,7 @@
         <v/>
       </c>
     </row>
-    <row r="408" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="408" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A408" s="8"/>
       <c r="B408" s="8"/>
       <c r="C408" s="8"/>
@@ -26975,7 +26971,7 @@
         <v/>
       </c>
     </row>
-    <row r="409" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="409" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A409" s="8"/>
       <c r="B409" s="8"/>
       <c r="C409" s="8"/>
@@ -27029,7 +27025,7 @@
         <v/>
       </c>
     </row>
-    <row r="410" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="410" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A410" s="8"/>
       <c r="B410" s="8"/>
       <c r="C410" s="8"/>
@@ -27083,7 +27079,7 @@
         <v/>
       </c>
     </row>
-    <row r="411" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="411" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A411" s="8"/>
       <c r="B411" s="8"/>
       <c r="C411" s="8"/>
@@ -27137,7 +27133,7 @@
         <v/>
       </c>
     </row>
-    <row r="412" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="412" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A412" s="8"/>
       <c r="B412" s="8"/>
       <c r="C412" s="8"/>
@@ -27191,7 +27187,7 @@
         <v/>
       </c>
     </row>
-    <row r="413" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="413" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A413" s="8"/>
       <c r="B413" s="8"/>
       <c r="C413" s="8"/>
@@ -27245,7 +27241,7 @@
         <v/>
       </c>
     </row>
-    <row r="414" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="414" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A414" s="8"/>
       <c r="B414" s="8"/>
       <c r="C414" s="8"/>
@@ -27299,7 +27295,7 @@
         <v/>
       </c>
     </row>
-    <row r="415" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="415" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A415" s="8"/>
       <c r="B415" s="8"/>
       <c r="C415" s="8"/>
@@ -27353,7 +27349,7 @@
         <v/>
       </c>
     </row>
-    <row r="416" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="416" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A416" s="8"/>
       <c r="B416" s="8"/>
       <c r="C416" s="8"/>
@@ -27407,7 +27403,7 @@
         <v/>
       </c>
     </row>
-    <row r="417" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="417" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A417" s="8"/>
       <c r="B417" s="8"/>
       <c r="C417" s="8"/>
@@ -27461,7 +27457,7 @@
         <v/>
       </c>
     </row>
-    <row r="418" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="418" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A418" s="8"/>
       <c r="B418" s="8"/>
       <c r="C418" s="8"/>
@@ -27515,7 +27511,7 @@
         <v/>
       </c>
     </row>
-    <row r="419" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="419" spans="1:19" x14ac:dyDescent="0.4">
       <c r="I419" s="13" t="str">
         <f t="shared" si="66"/>
         <v/>
@@ -27562,7 +27558,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="BqKaXR7gwV4fXkT/peGRFL6ybIBaxli5Aqp5eDZbOLGuzrWjuU+y5r2sA00HggCFyyQDQ15A8LpAac/MF5HuRg==" saltValue="RJT7Dp/NNVsZ2UODI2NGYQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="d8GAWrcylpRAU9Bzft9v/zA9KVKsn2S6bN9BcAsL/4LXTx70NRd+TDAtytgDT7tGcH0vTK0CNMgka/LCvVsa1A==" saltValue="/EmZVIMXB78xBDDfHdnMvw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="I1:S1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>
@@ -27590,192 +27586,192 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="102" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
feat: disable waterpoins layer LSO AB#34472
</commit_message>
<xml_diff>
--- a/services/API-service/src/scripts/json/layer-popup-info.xlsx
+++ b/services/API-service/src/scripts/json/layer-popup-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\IBF-system\services\API-service\src\scripts\json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F897946-65C6-4FE1-9B44-FAE99E2743C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4689B85-5BEE-47DF-AD9B-424AB6D79AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57360" yWindow="-9300" windowWidth="29280" windowHeight="15960" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
+    <workbookView xWindow="-48" yWindow="-48" windowWidth="23136" windowHeight="13776" xr2:uid="{596CF045-89F9-477C-A1A6-2B5E1A5402AC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="267">
   <si>
     <t>section</t>
   </si>
@@ -1284,8 +1284,8 @@
   <dimension ref="A1:P400"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E205" sqref="E205"/>
+      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E204" sqref="E204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -13407,7 +13407,7 @@
         <v>"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source Link: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="4" t="s">
         <v>81</v>
       </c>
@@ -13415,13 +13415,13 @@
         <v>25</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>265</v>
+        <v>24</v>
       </c>
       <c r="D200" s="4" t="s">
         <v>103</v>
       </c>
       <c r="E200" s="3" t="s">
-        <v>50</v>
+        <v>258</v>
       </c>
       <c r="F200" s="8" t="str">
         <f t="shared" si="33"/>
@@ -13437,19 +13437,19 @@
       </c>
       <c r="I200" s="12" t="str">
         <f t="shared" si="36"/>
-        <v>"LSO": {</v>
+        <v>"ZMB": {</v>
       </c>
       <c r="J200" s="7" t="str">
         <f t="shared" si="37"/>
-        <v>"drought": "TBD"</v>
+        <v>"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"</v>
       </c>
       <c r="K200" s="13" t="str">
         <f t="shared" si="38"/>
-        <v>}</v>
+        <v>,</v>
       </c>
       <c r="L200" s="7" t="str">
         <f t="shared" si="39"/>
-        <v>,</v>
+        <v/>
       </c>
       <c r="M200" s="7" t="str">
         <f t="shared" si="40"/>
@@ -13465,7 +13465,7 @@
       </c>
       <c r="P200" s="7" t="str">
         <f t="shared" si="43"/>
-        <v>"LSO": {"drought": "TBD"},</v>
+        <v>"ZMB": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;",</v>
       </c>
     </row>
     <row r="201" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -13479,7 +13479,7 @@
         <v>24</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>258</v>
@@ -13498,19 +13498,19 @@
       </c>
       <c r="I201" s="12" t="str">
         <f t="shared" si="36"/>
-        <v>"ZMB": {</v>
+        <v/>
       </c>
       <c r="J201" s="7" t="str">
         <f t="shared" si="37"/>
-        <v>"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"</v>
+        <v>"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"</v>
       </c>
       <c r="K201" s="13" t="str">
         <f t="shared" si="38"/>
-        <v>,</v>
+        <v>}</v>
       </c>
       <c r="L201" s="7" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>,</v>
       </c>
       <c r="M201" s="7" t="str">
         <f t="shared" si="40"/>
@@ -13526,7 +13526,7 @@
       </c>
       <c r="P201" s="7" t="str">
         <f t="shared" si="43"/>
-        <v>"ZMB": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;",</v>
+        <v>"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
       </c>
     </row>
     <row r="202" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -13537,10 +13537,10 @@
         <v>25</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D202" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>258</v>
@@ -13559,11 +13559,11 @@
       </c>
       <c r="I202" s="12" t="str">
         <f t="shared" si="36"/>
-        <v/>
+        <v>"ZWE": {</v>
       </c>
       <c r="J202" s="7" t="str">
         <f t="shared" si="37"/>
-        <v>"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"</v>
+        <v>"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"</v>
       </c>
       <c r="K202" s="13" t="str">
         <f t="shared" si="38"/>
@@ -13571,11 +13571,11 @@
       </c>
       <c r="L202" s="7" t="str">
         <f t="shared" si="39"/>
-        <v>,</v>
+        <v>}</v>
       </c>
       <c r="M202" s="7" t="str">
         <f t="shared" si="40"/>
-        <v/>
+        <v>,</v>
       </c>
       <c r="N202" s="7" t="str">
         <f t="shared" si="41"/>
@@ -13587,24 +13587,24 @@
       </c>
       <c r="P202" s="7" t="str">
         <f t="shared" si="43"/>
-        <v>"floods": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"},</v>
-      </c>
-    </row>
-    <row r="203" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>"ZWE": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"}},</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>25</v>
+        <v>138</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="D203" s="4" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="E203" s="3" t="s">
-        <v>258</v>
+        <v>50</v>
       </c>
       <c r="F203" s="8" t="str">
         <f t="shared" si="33"/>
@@ -13616,15 +13616,15 @@
       </c>
       <c r="H203" s="7" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>"waterpoints_internal": {</v>
       </c>
       <c r="I203" s="12" t="str">
         <f t="shared" si="36"/>
-        <v>"ZWE": {</v>
+        <v>"MWI": {</v>
       </c>
       <c r="J203" s="7" t="str">
         <f t="shared" si="37"/>
-        <v>"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"</v>
+        <v>"flash-floods": "TBD"</v>
       </c>
       <c r="K203" s="13" t="str">
         <f t="shared" si="38"/>
@@ -13648,24 +13648,24 @@
       </c>
       <c r="P203" s="7" t="str">
         <f t="shared" si="43"/>
-        <v>"ZWE": {"drought": "Number and location of functioning waterpoints accessible for people (Borehole, Protected Spring, Protected Shallow Well, Rainwater Harvesting, Sand or Sub-surface Dam, Spring, Surface Water, Undefined Shallow Well, Undefined Well, Unprotected Shallow Well).&lt;br/&gt;&lt;br/&gt;Source: &lt;a href='https://www.waterpointdata.org/water-point-data'&gt;https://www.waterpointdata.org/water-point-data&lt;/a&gt;"}},</v>
-      </c>
-    </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>"waterpoints_internal": {"MWI": {"flash-floods": "TBD"}},</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="D204" s="4" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="E204" s="3" t="s">
-        <v>50</v>
+        <v>260</v>
       </c>
       <c r="F204" s="8" t="str">
         <f t="shared" si="33"/>
@@ -13677,15 +13677,15 @@
       </c>
       <c r="H204" s="7" t="str">
         <f t="shared" si="35"/>
-        <v>"waterpoints_internal": {</v>
+        <v>"windspeed": {</v>
       </c>
       <c r="I204" s="12" t="str">
         <f t="shared" si="36"/>
-        <v>"MWI": {</v>
+        <v>"PHL": {</v>
       </c>
       <c r="J204" s="7" t="str">
         <f t="shared" si="37"/>
-        <v>"flash-floods": "TBD"</v>
+        <v>"typhoon": "Forecasted 1 minute average maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event.&lt;br/&gt;&lt;br/&gt;Source (Typhoon Forecast): ECMWF"</v>
       </c>
       <c r="K204" s="13" t="str">
         <f t="shared" si="38"/>
@@ -13697,64 +13697,54 @@
       </c>
       <c r="M204" s="7" t="str">
         <f t="shared" si="40"/>
-        <v>,</v>
+        <v/>
       </c>
       <c r="N204" s="7" t="str">
         <f t="shared" si="41"/>
-        <v/>
+        <v>}</v>
       </c>
       <c r="O204" s="7" t="str">
         <f t="shared" si="42"/>
-        <v/>
+        <v>}</v>
       </c>
       <c r="P204" s="7" t="str">
         <f t="shared" si="43"/>
-        <v>"waterpoints_internal": {"MWI": {"flash-floods": "TBD"}},</v>
-      </c>
-    </row>
-    <row r="205" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A205" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B205" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C205" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D205" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E205" s="3" t="s">
-        <v>260</v>
-      </c>
+        <v>"windspeed": {"PHL": {"typhoon": "Forecasted 1 minute average maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event.&lt;br/&gt;&lt;br/&gt;Source (Typhoon Forecast): ECMWF"}}}}</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A205" s="4"/>
+      <c r="B205" s="4"/>
+      <c r="C205" s="4"/>
+      <c r="D205" s="4"/>
+      <c r="E205" s="3"/>
       <c r="F205" s="8" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="G205" s="7" t="str">
         <f t="shared" si="34"/>
-        <v/>
+        <v>"": {</v>
       </c>
       <c r="H205" s="7" t="str">
         <f t="shared" si="35"/>
-        <v>"windspeed": {</v>
+        <v>"": {</v>
       </c>
       <c r="I205" s="12" t="str">
         <f t="shared" si="36"/>
-        <v>"PHL": {</v>
+        <v>"": {</v>
       </c>
       <c r="J205" s="7" t="str">
         <f t="shared" si="37"/>
-        <v>"typhoon": "Forecasted 1 minute average maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event.&lt;br/&gt;&lt;br/&gt;Source (Typhoon Forecast): ECMWF"</v>
+        <v>"": ""</v>
       </c>
       <c r="K205" s="13" t="str">
         <f t="shared" si="38"/>
-        <v>}</v>
+        <v>,</v>
       </c>
       <c r="L205" s="7" t="str">
         <f t="shared" si="39"/>
-        <v>}</v>
+        <v/>
       </c>
       <c r="M205" s="7" t="str">
         <f t="shared" si="40"/>
@@ -13762,7 +13752,7 @@
       </c>
       <c r="N205" s="7" t="str">
         <f t="shared" si="41"/>
-        <v>}</v>
+        <v/>
       </c>
       <c r="O205" s="7" t="str">
         <f t="shared" si="42"/>
@@ -13770,7 +13760,7 @@
       </c>
       <c r="P205" s="7" t="str">
         <f t="shared" si="43"/>
-        <v>"windspeed": {"PHL": {"typhoon": "Forecasted 1 minute average maximum wind speed in kilometers per hour for each municipality during the duration of the typhoon event.&lt;br/&gt;&lt;br/&gt;Source (Typhoon Forecast): ECMWF"}}}}</v>
+        <v/>
       </c>
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -13785,15 +13775,15 @@
       </c>
       <c r="G206" s="7" t="str">
         <f t="shared" si="34"/>
-        <v>"": {</v>
+        <v/>
       </c>
       <c r="H206" s="7" t="str">
         <f t="shared" si="35"/>
-        <v>"": {</v>
+        <v/>
       </c>
       <c r="I206" s="12" t="str">
         <f t="shared" si="36"/>
-        <v>"": {</v>
+        <v/>
       </c>
       <c r="J206" s="7" t="str">
         <f t="shared" si="37"/>
@@ -23714,7 +23704,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="oNTLlLfOHkBtP51iKKzmEUXOHzxYMLbegJRH8kYICVpDnzyKq7xpKh851VrujcsrrDk/QFnl/zE3BGKzWMxRgQ==" saltValue="0/nqL2PoZGXLPuxN8o62BQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="hXFPKznllUPnr9FpmQeQO/78tsGRB8QK+V3j27t4PhcCen0FRJG6YpYSnHCUQCD+NYkrSKMsSlF8GqPBcHMBOg==" saltValue="EJ6uUmiy2JirvKxWz7Vhrg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="NgPY829S+ohHrwctHQLUGnVp3aC/FbhMzlJhwokHCOi1dJ0uiHIV2+J3q0P23C8LIgG8AOIg5kXPTZ28z8FMag==" saltValue="pkVAOC3cVOjDXjOHQJWN6w==" spinCount="100000" sqref="F1:P1048576" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="eCfXFnSEnhvW0qovVEYMUlzR0+k9pUf39l1PN6i4hlKfXGzore6xz/ntoKarV0I55jiM5pq3izZlv1hIi9y5MQ==" saltValue="LlQbkbA4ALZMlj/SyzLWNw==" spinCount="100000" sqref="A1:XFD1" name="Range2"/>

</xml_diff>